<commit_message>
fix program listing pdf links
</commit_message>
<xml_diff>
--- a/static/programlisting.xlsx
+++ b/static/programlisting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\aolccbc.com\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7369565-763D-4404-AF60-CF2F6704B3B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB5BD0C-7930-4645-AFF4-7DA68E7C425D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -722,59 +722,59 @@
       <sheetName val="Reference"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-      <sheetData sheetId="52" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
+      <sheetData sheetId="51"/>
+      <sheetData sheetId="52"/>
       <sheetData sheetId="53">
         <row r="5">
           <cell r="A5" t="str">
@@ -2047,8 +2047,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="55" refreshError="1"/>
-      <sheetData sheetId="56" refreshError="1"/>
+      <sheetData sheetId="55"/>
+      <sheetData sheetId="56"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2353,8 +2353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2419,11 +2419,11 @@
         <v>A+ Network+ And Mcsa Desktop Cert. Prep</v>
       </c>
       <c r="B2" s="1">
-        <f t="shared" ref="B2:B33" ca="1" si="0">C2/weeks</f>
+        <f t="shared" ref="B2:B33" si="0">C2/weeks</f>
         <v>34.090909090909093</v>
       </c>
       <c r="C2" s="1">
-        <f ca="1">[1]Summary!$G5</f>
+        <f>[1]Summary!$G5</f>
         <v>750</v>
       </c>
       <c r="D2" t="s">
@@ -2437,7 +2437,7 @@
         <v>Certificate</v>
       </c>
       <c r="G2">
-        <f ca="1">[1]Summary!$H5</f>
+        <f>[1]Summary!$H5</f>
         <v>8510</v>
       </c>
       <c r="H2" t="s">
@@ -2469,11 +2469,11 @@
         <v>Accounting Administrator Diploma With Sage</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>35.863636363636367</v>
       </c>
       <c r="C3" s="1">
-        <f ca="1">[1]Summary!$G6</f>
+        <f>[1]Summary!$G6</f>
         <v>789</v>
       </c>
       <c r="D3" t="s">
@@ -2487,7 +2487,7 @@
         <v>Diploma</v>
       </c>
       <c r="G3">
-        <f ca="1">[1]Summary!$H6</f>
+        <f>[1]Summary!$H6</f>
         <v>11559</v>
       </c>
       <c r="H3" t="s">
@@ -2509,8 +2509,8 @@
         <v>accounting_administrator_with_sage_programdata.json</v>
       </c>
       <c r="N3" t="str">
-        <f t="shared" ref="N3:N51" si="4">_xlfn.CONCAT(L3,".pdf")</f>
-        <v>accounting_administrator_with_sage.pdf</v>
+        <f t="shared" ref="N3:N52" si="4">_xlfn.CONCAT(L3,"_",LOWER(F3),".pdf")</f>
+        <v>accounting_administrator_with_sage_diploma.pdf</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2519,11 +2519,11 @@
         <v>Accounting And Business Technology Diploma</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>40.863636363636367</v>
       </c>
       <c r="C4" s="1">
-        <f ca="1">[1]Summary!$G7</f>
+        <f>[1]Summary!$G7</f>
         <v>899</v>
       </c>
       <c r="D4" t="s">
@@ -2537,7 +2537,7 @@
         <v>Diploma</v>
       </c>
       <c r="G4">
-        <f ca="1">[1]Summary!$H7</f>
+        <f>[1]Summary!$H7</f>
         <v>12729</v>
       </c>
       <c r="H4" t="s">
@@ -2560,7 +2560,7 @@
       </c>
       <c r="N4" t="str">
         <f t="shared" si="4"/>
-        <v>accounting_and_business_technology.pdf</v>
+        <v>accounting_and_business_technology_diploma.pdf</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -2569,11 +2569,11 @@
         <v>Accounting And Payroll Administrator Diploma</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>49.272727272727273</v>
       </c>
       <c r="C5" s="1">
-        <f ca="1">[1]Summary!$G8</f>
+        <f>[1]Summary!$G8</f>
         <v>1084</v>
       </c>
       <c r="D5" t="s">
@@ -2587,7 +2587,7 @@
         <v>Diploma</v>
       </c>
       <c r="G5">
-        <f ca="1">[1]Summary!$H8</f>
+        <f>[1]Summary!$H8</f>
         <v>15180</v>
       </c>
       <c r="H5" t="s">
@@ -2610,7 +2610,7 @@
       </c>
       <c r="N5" t="str">
         <f t="shared" si="4"/>
-        <v>accounting_and_payroll_administrator.pdf</v>
+        <v>accounting_and_payroll_administrator_diploma.pdf</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -2619,11 +2619,11 @@
         <v>Accounting Bookkeeper Certificate</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>29.227272727272727</v>
       </c>
       <c r="C6" s="1">
-        <f ca="1">[1]Summary!$G9</f>
+        <f>[1]Summary!$G9</f>
         <v>643</v>
       </c>
       <c r="D6" t="s">
@@ -2637,7 +2637,7 @@
         <v>Certificate</v>
       </c>
       <c r="G6">
-        <f ca="1">[1]Summary!$H9</f>
+        <f>[1]Summary!$H9</f>
         <v>8707</v>
       </c>
       <c r="H6" t="s">
@@ -2660,7 +2660,7 @@
       </c>
       <c r="N6" t="str">
         <f t="shared" si="4"/>
-        <v>accounting_bookkeeper.pdf</v>
+        <v>accounting_bookkeeper_certificate.pdf</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -2669,11 +2669,11 @@
         <v>Accounting Clerk Certificate</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>20.90909090909091</v>
       </c>
       <c r="C7" s="1">
-        <f ca="1">[1]Summary!$G10</f>
+        <f>[1]Summary!$G10</f>
         <v>460</v>
       </c>
       <c r="D7" t="s">
@@ -2687,7 +2687,7 @@
         <v>Certificate</v>
       </c>
       <c r="G7">
-        <f ca="1">[1]Summary!$H10</f>
+        <f>[1]Summary!$H10</f>
         <v>6452</v>
       </c>
       <c r="H7" t="s">
@@ -2710,7 +2710,7 @@
       </c>
       <c r="N7" t="str">
         <f t="shared" si="4"/>
-        <v>accounting_clerk.pdf</v>
+        <v>accounting_clerk_certificate.pdf</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -2719,11 +2719,11 @@
         <v>Addictions Worker Certificate</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>13.636363636363637</v>
       </c>
       <c r="C8" s="1">
-        <f ca="1">[1]Summary!$G11</f>
+        <f>[1]Summary!$G11</f>
         <v>300</v>
       </c>
       <c r="D8" t="s">
@@ -2737,7 +2737,7 @@
         <v>Certificate</v>
       </c>
       <c r="G8">
-        <f ca="1">[1]Summary!$H11</f>
+        <f>[1]Summary!$H11</f>
         <v>3079</v>
       </c>
       <c r="H8" t="s">
@@ -2760,7 +2760,7 @@
       </c>
       <c r="N8" t="str">
         <f t="shared" si="4"/>
-        <v>addictions_worker.pdf</v>
+        <v>addictions_worker_certificate.pdf</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -2769,11 +2769,11 @@
         <v>Administrative Assistant Diploma</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>34.909090909090907</v>
       </c>
       <c r="C9" s="1">
-        <f ca="1">[1]Summary!$G12</f>
+        <f>[1]Summary!$G12</f>
         <v>768</v>
       </c>
       <c r="D9" t="s">
@@ -2787,7 +2787,7 @@
         <v>Diploma</v>
       </c>
       <c r="G9">
-        <f ca="1">[1]Summary!$H12</f>
+        <f>[1]Summary!$H12</f>
         <v>10097</v>
       </c>
       <c r="H9" t="s">
@@ -2810,7 +2810,7 @@
       </c>
       <c r="N9" t="str">
         <f t="shared" si="4"/>
-        <v>administrative_assistant.pdf</v>
+        <v>administrative_assistant_diploma.pdf</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -2819,11 +2819,11 @@
         <v>Business Administration Co-Op Diploma</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>6.4090909090909092</v>
       </c>
       <c r="C10" s="1">
-        <f ca="1">[1]Summary!$G13</f>
+        <f>[1]Summary!$G13</f>
         <v>141</v>
       </c>
       <c r="D10" t="s">
@@ -2837,7 +2837,7 @@
         <v>Diploma</v>
       </c>
       <c r="G10">
-        <f ca="1">[1]Summary!$H13</f>
+        <f>[1]Summary!$H13</f>
         <v>22293</v>
       </c>
       <c r="H10" t="s">
@@ -2860,7 +2860,7 @@
       </c>
       <c r="N10" t="str">
         <f t="shared" si="4"/>
-        <v>business_administration_co_op.pdf</v>
+        <v>business_administration_co_op_diploma.pdf</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -2869,11 +2869,11 @@
         <v>Business Administration Diploma</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>6.1818181818181817</v>
       </c>
       <c r="C11" s="1">
-        <f ca="1">[1]Summary!$G14</f>
+        <f>[1]Summary!$G14</f>
         <v>136</v>
       </c>
       <c r="D11" t="s">
@@ -2887,7 +2887,7 @@
         <v>Diploma</v>
       </c>
       <c r="G11">
-        <f ca="1">[1]Summary!$H14</f>
+        <f>[1]Summary!$H14</f>
         <v>17893</v>
       </c>
       <c r="H11" t="s">
@@ -2910,7 +2910,7 @@
       </c>
       <c r="N11" t="str">
         <f t="shared" si="4"/>
-        <v>business_administration.pdf</v>
+        <v>business_administration_diploma.pdf</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -2919,11 +2919,11 @@
         <v>Business Management Certificate</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>28.045454545454547</v>
       </c>
       <c r="C12" s="1">
-        <f ca="1">[1]Summary!$G15</f>
+        <f>[1]Summary!$G15</f>
         <v>617</v>
       </c>
       <c r="D12" t="s">
@@ -2937,7 +2937,7 @@
         <v>Certificate</v>
       </c>
       <c r="G12">
-        <f ca="1">[1]Summary!$H15</f>
+        <f>[1]Summary!$H15</f>
         <v>9329</v>
       </c>
       <c r="H12" t="s">
@@ -2960,7 +2960,7 @@
       </c>
       <c r="N12" t="str">
         <f t="shared" si="4"/>
-        <v>business_management.pdf</v>
+        <v>business_management_certificate.pdf</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -2969,11 +2969,11 @@
         <v>Business Office Skills Diploma</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>38.31818181818182</v>
       </c>
       <c r="C13" s="1">
-        <f ca="1">[1]Summary!$G16</f>
+        <f>[1]Summary!$G16</f>
         <v>843</v>
       </c>
       <c r="D13" t="s">
@@ -2987,7 +2987,7 @@
         <v>Diploma</v>
       </c>
       <c r="G13">
-        <f ca="1">[1]Summary!$H16</f>
+        <f>[1]Summary!$H16</f>
         <v>11409</v>
       </c>
       <c r="H13" t="s">
@@ -3010,7 +3010,7 @@
       </c>
       <c r="N13" t="str">
         <f t="shared" si="4"/>
-        <v>business_office_skills.pdf</v>
+        <v>business_office_skills_diploma.pdf</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -3019,11 +3019,11 @@
         <v>Business Receptionist Certificate</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>24.59090909090909</v>
       </c>
       <c r="C14" s="1">
-        <f ca="1">[1]Summary!$G17</f>
+        <f>[1]Summary!$G17</f>
         <v>541</v>
       </c>
       <c r="D14" t="s">
@@ -3037,7 +3037,7 @@
         <v>Certificate</v>
       </c>
       <c r="G14">
-        <f ca="1">[1]Summary!$H17</f>
+        <f>[1]Summary!$H17</f>
         <v>7135</v>
       </c>
       <c r="H14" t="s">
@@ -3060,7 +3060,7 @@
       </c>
       <c r="N14" t="str">
         <f t="shared" si="4"/>
-        <v>business_receptionist.pdf</v>
+        <v>business_receptionist_certificate.pdf</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -3069,11 +3069,11 @@
         <v>Business Service Essentials Co-Op Diploma</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>48.909090909090907</v>
       </c>
       <c r="C15" s="1">
-        <f ca="1">[1]Summary!$G18</f>
+        <f>[1]Summary!$G18</f>
         <v>1076</v>
       </c>
       <c r="D15" t="s">
@@ -3087,7 +3087,7 @@
         <v>Diploma</v>
       </c>
       <c r="G15">
-        <f ca="1">[1]Summary!$H18</f>
+        <f>[1]Summary!$H18</f>
         <v>10752</v>
       </c>
       <c r="H15" t="s">
@@ -3110,7 +3110,7 @@
       </c>
       <c r="N15" t="str">
         <f t="shared" si="4"/>
-        <v>business_service_essentials_co_op.pdf</v>
+        <v>business_service_essentials_co_op_diploma.pdf</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -3119,11 +3119,11 @@
         <v>Call Centre Customer Representative Diploma</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>31.181818181818183</v>
       </c>
       <c r="C16" s="1">
-        <f ca="1">[1]Summary!$G19</f>
+        <f>[1]Summary!$G19</f>
         <v>686</v>
       </c>
       <c r="D16" t="s">
@@ -3137,7 +3137,7 @@
         <v>Diploma</v>
       </c>
       <c r="G16">
-        <f ca="1">[1]Summary!$H19</f>
+        <f>[1]Summary!$H19</f>
         <v>9627</v>
       </c>
       <c r="H16" t="s">
@@ -3160,7 +3160,7 @@
       </c>
       <c r="N16" t="str">
         <f t="shared" si="4"/>
-        <v>call_centre_customer_representative.pdf</v>
+        <v>call_centre_customer_representative_diploma.pdf</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -3169,11 +3169,11 @@
         <v>Community Service Worker And Addictions Worker Diploma</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>52.590909090909093</v>
       </c>
       <c r="C17" s="1">
-        <f ca="1">[1]Summary!$G20</f>
+        <f>[1]Summary!$G20</f>
         <v>1157</v>
       </c>
       <c r="D17" t="s">
@@ -3187,7 +3187,7 @@
         <v>Diploma</v>
       </c>
       <c r="G17">
-        <f ca="1">[1]Summary!$H20</f>
+        <f>[1]Summary!$H20</f>
         <v>15449</v>
       </c>
       <c r="H17" t="s">
@@ -3210,7 +3210,7 @@
       </c>
       <c r="N17" t="str">
         <f t="shared" si="4"/>
-        <v>community_service_worker_and_addictions_worker.pdf</v>
+        <v>community_service_worker_and_addictions_worker_diploma.pdf</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -3219,11 +3219,11 @@
         <v>Community Service Worker Diploma</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>37.590909090909093</v>
       </c>
       <c r="C18" s="1">
-        <f ca="1">[1]Summary!$G21</f>
+        <f>[1]Summary!$G21</f>
         <v>827</v>
       </c>
       <c r="D18" t="s">
@@ -3237,7 +3237,7 @@
         <v>Diploma</v>
       </c>
       <c r="G18">
-        <f ca="1">[1]Summary!$H21</f>
+        <f>[1]Summary!$H21</f>
         <v>12370</v>
       </c>
       <c r="H18" t="s">
@@ -3260,7 +3260,7 @@
       </c>
       <c r="N18" t="str">
         <f t="shared" si="4"/>
-        <v>community_service_worker.pdf</v>
+        <v>community_service_worker_diploma.pdf</v>
       </c>
       <c r="O18" t="s">
         <v>18</v>
@@ -3272,11 +3272,11 @@
         <v>Computer Service Technician Certificate</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>26.636363636363637</v>
       </c>
       <c r="C19" s="1">
-        <f ca="1">[1]Summary!$G22</f>
+        <f>[1]Summary!$G22</f>
         <v>586</v>
       </c>
       <c r="D19" t="s">
@@ -3290,7 +3290,7 @@
         <v>Certificate</v>
       </c>
       <c r="G19">
-        <f ca="1">[1]Summary!$H22</f>
+        <f>[1]Summary!$H22</f>
         <v>5822</v>
       </c>
       <c r="H19" t="s">
@@ -3316,7 +3316,7 @@
       </c>
       <c r="N19" t="str">
         <f t="shared" si="4"/>
-        <v>computer_service_technician_c.pdf</v>
+        <v>computer_service_technician_c_certificate.pdf</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -3325,11 +3325,11 @@
         <v>Computer Service Technician Diploma</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>46.31818181818182</v>
       </c>
       <c r="C20" s="1">
-        <f ca="1">[1]Summary!$G23</f>
+        <f>[1]Summary!$G23</f>
         <v>1019</v>
       </c>
       <c r="D20" t="s">
@@ -3343,7 +3343,7 @@
         <v>Diploma</v>
       </c>
       <c r="G20">
-        <f ca="1">[1]Summary!$H23</f>
+        <f>[1]Summary!$H23</f>
         <v>12167</v>
       </c>
       <c r="H20" t="s">
@@ -3369,7 +3369,7 @@
       </c>
       <c r="N20" t="str">
         <f t="shared" si="4"/>
-        <v>computer_service_technician_d.pdf</v>
+        <v>computer_service_technician_d_diploma.pdf</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -3378,11 +3378,11 @@
         <v>Computer Software Support Diploma</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>46.31818181818182</v>
       </c>
       <c r="C21" s="1">
-        <f ca="1">[1]Summary!$G24</f>
+        <f>[1]Summary!$G24</f>
         <v>1019</v>
       </c>
       <c r="D21" t="s">
@@ -3396,7 +3396,7 @@
         <v>Diploma</v>
       </c>
       <c r="G21">
-        <f ca="1">[1]Summary!$H24</f>
+        <f>[1]Summary!$H24</f>
         <v>12167</v>
       </c>
       <c r="H21" t="s">
@@ -3419,7 +3419,7 @@
       </c>
       <c r="N21" t="str">
         <f t="shared" si="4"/>
-        <v>computer_software_support.pdf</v>
+        <v>computer_software_support_diploma.pdf</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -3428,11 +3428,11 @@
         <v>Computerized Office Procedures Certificate</v>
       </c>
       <c r="B22" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>25.59090909090909</v>
       </c>
       <c r="C22" s="1">
-        <f ca="1">[1]Summary!$G25</f>
+        <f>[1]Summary!$G25</f>
         <v>563</v>
       </c>
       <c r="D22" t="s">
@@ -3446,7 +3446,7 @@
         <v>Certificate</v>
       </c>
       <c r="G22">
-        <f ca="1">[1]Summary!$H25</f>
+        <f>[1]Summary!$H25</f>
         <v>7132</v>
       </c>
       <c r="H22" t="s">
@@ -3469,7 +3469,7 @@
       </c>
       <c r="N22" t="str">
         <f t="shared" si="4"/>
-        <v>computerized_office_procedures.pdf</v>
+        <v>computerized_office_procedures_certificate.pdf</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -3478,11 +3478,11 @@
         <v>Conference And Event Planner Diploma</v>
       </c>
       <c r="B23" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>46.227272727272727</v>
       </c>
       <c r="C23" s="1">
-        <f ca="1">[1]Summary!$G26</f>
+        <f>[1]Summary!$G26</f>
         <v>1017</v>
       </c>
       <c r="D23" t="s">
@@ -3496,7 +3496,7 @@
         <v>Diploma</v>
       </c>
       <c r="G23">
-        <f ca="1">[1]Summary!$H26</f>
+        <f>[1]Summary!$H26</f>
         <v>14474</v>
       </c>
       <c r="H23" t="s">
@@ -3519,7 +3519,7 @@
       </c>
       <c r="N23" t="str">
         <f t="shared" si="4"/>
-        <v>conference_and_event_planner.pdf</v>
+        <v>conference_and_event_planner_diploma.pdf</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -3528,11 +3528,11 @@
         <v>Customer Service Representative Certificate</v>
       </c>
       <c r="B24" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>20.727272727272727</v>
       </c>
       <c r="C24" s="1">
-        <f ca="1">[1]Summary!$G27</f>
+        <f>[1]Summary!$G27</f>
         <v>456</v>
       </c>
       <c r="D24" t="s">
@@ -3546,7 +3546,7 @@
         <v>Certificate</v>
       </c>
       <c r="G24">
-        <f ca="1">[1]Summary!$H27</f>
+        <f>[1]Summary!$H27</f>
         <v>6271</v>
       </c>
       <c r="H24" t="s">
@@ -3569,7 +3569,7 @@
       </c>
       <c r="N24" t="str">
         <f t="shared" si="4"/>
-        <v>customer_service_representative.pdf</v>
+        <v>customer_service_representative_certificate.pdf</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -3578,11 +3578,11 @@
         <v>English As Second Language</v>
       </c>
       <c r="B25" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>14.545454545454545</v>
       </c>
       <c r="C25" s="1">
-        <f ca="1">[1]Summary!$G28</f>
+        <f>[1]Summary!$G28</f>
         <v>320</v>
       </c>
       <c r="D25" t="s">
@@ -3596,7 +3596,7 @@
         <v>Certificate</v>
       </c>
       <c r="G25">
-        <f ca="1">[1]Summary!$H28</f>
+        <f>[1]Summary!$H28</f>
         <v>3390</v>
       </c>
       <c r="H25" t="s">
@@ -3619,7 +3619,7 @@
       </c>
       <c r="N25" t="str">
         <f t="shared" si="4"/>
-        <v>english_as_second_language.pdf</v>
+        <v>english_as_second_language_certificate.pdf</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -3628,11 +3628,11 @@
         <v>Entrepreneurial Business Applications Diploma</v>
       </c>
       <c r="B26" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>41.18181818181818</v>
       </c>
       <c r="C26" s="1">
-        <f ca="1">[1]Summary!$G29</f>
+        <f>[1]Summary!$G29</f>
         <v>906</v>
       </c>
       <c r="D26" t="s">
@@ -3646,7 +3646,7 @@
         <v>Diploma</v>
       </c>
       <c r="G26">
-        <f ca="1">[1]Summary!$H29</f>
+        <f>[1]Summary!$H29</f>
         <v>12541</v>
       </c>
       <c r="H26" t="s">
@@ -3669,7 +3669,7 @@
       </c>
       <c r="N26" t="str">
         <f t="shared" si="4"/>
-        <v>entrepreneurial_business_applications.pdf</v>
+        <v>entrepreneurial_business_applications_diploma.pdf</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -3678,11 +3678,11 @@
         <v>Executive Assistant Diploma</v>
       </c>
       <c r="B27" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>48.136363636363633</v>
       </c>
       <c r="C27" s="1">
-        <f ca="1">[1]Summary!$G30</f>
+        <f>[1]Summary!$G30</f>
         <v>1059</v>
       </c>
       <c r="D27" t="s">
@@ -3696,7 +3696,7 @@
         <v>Diploma</v>
       </c>
       <c r="G27">
-        <f ca="1">[1]Summary!$H30</f>
+        <f>[1]Summary!$H30</f>
         <v>14334</v>
       </c>
       <c r="H27" t="s">
@@ -3719,7 +3719,7 @@
       </c>
       <c r="N27" t="str">
         <f t="shared" si="4"/>
-        <v>executive_assistant.pdf</v>
+        <v>executive_assistant_diploma.pdf</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -3728,11 +3728,11 @@
         <v>Graphic Designer Diploma</v>
       </c>
       <c r="B28" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>49.454545454545453</v>
       </c>
       <c r="C28" s="1">
-        <f ca="1">[1]Summary!$G31</f>
+        <f>[1]Summary!$G31</f>
         <v>1088</v>
       </c>
       <c r="D28" t="s">
@@ -3746,7 +3746,7 @@
         <v>Diploma</v>
       </c>
       <c r="G28">
-        <f ca="1">[1]Summary!$H31</f>
+        <f>[1]Summary!$H31</f>
         <v>16396</v>
       </c>
       <c r="H28" t="s">
@@ -3769,7 +3769,7 @@
       </c>
       <c r="N28" t="str">
         <f t="shared" si="4"/>
-        <v>graphic_designer.pdf</v>
+        <v>graphic_designer_diploma.pdf</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -3778,11 +3778,11 @@
         <v>Human Resources Administration Certificate</v>
       </c>
       <c r="B29" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>29.09090909090909</v>
       </c>
       <c r="C29" s="1">
-        <f ca="1">[1]Summary!$G32</f>
+        <f>[1]Summary!$G32</f>
         <v>640</v>
       </c>
       <c r="D29" t="s">
@@ -3796,7 +3796,7 @@
         <v>Certificate</v>
       </c>
       <c r="G29">
-        <f ca="1">[1]Summary!$H32</f>
+        <f>[1]Summary!$H32</f>
         <v>8468</v>
       </c>
       <c r="H29" t="s">
@@ -3819,7 +3819,7 @@
       </c>
       <c r="N29" t="str">
         <f t="shared" si="4"/>
-        <v>human_resources_administration.pdf</v>
+        <v>human_resources_administration_certificate.pdf</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -3828,11 +3828,11 @@
         <v>Marketing Administrative Assistant Certificate</v>
       </c>
       <c r="B30" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>34.545454545454547</v>
       </c>
       <c r="C30" s="1">
-        <f ca="1">[1]Summary!$G33</f>
+        <f>[1]Summary!$G33</f>
         <v>760</v>
       </c>
       <c r="D30" t="s">
@@ -3846,7 +3846,7 @@
         <v>Certificate</v>
       </c>
       <c r="G30">
-        <f ca="1">[1]Summary!$H33</f>
+        <f>[1]Summary!$H33</f>
         <v>10655</v>
       </c>
       <c r="H30" t="s">
@@ -3869,7 +3869,7 @@
       </c>
       <c r="N30" t="str">
         <f t="shared" si="4"/>
-        <v>marketing_administrative_assistant.pdf</v>
+        <v>marketing_administrative_assistant_certificate.pdf</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -3878,11 +3878,11 @@
         <v>Marketing Coordinator Diploma</v>
       </c>
       <c r="B31" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43.045454545454547</v>
       </c>
       <c r="C31" s="1">
-        <f ca="1">[1]Summary!$G34</f>
+        <f>[1]Summary!$G34</f>
         <v>947</v>
       </c>
       <c r="D31" t="s">
@@ -3896,7 +3896,7 @@
         <v>Diploma</v>
       </c>
       <c r="G31">
-        <f ca="1">[1]Summary!$H34</f>
+        <f>[1]Summary!$H34</f>
         <v>14242</v>
       </c>
       <c r="H31" t="s">
@@ -3919,7 +3919,7 @@
       </c>
       <c r="N31" t="str">
         <f t="shared" si="4"/>
-        <v>marketing_coordinator.pdf</v>
+        <v>marketing_coordinator_diploma.pdf</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -3928,11 +3928,11 @@
         <v>Medical Administrative Assistant Certificate</v>
       </c>
       <c r="B32" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>39.727272727272727</v>
       </c>
       <c r="C32" s="1">
-        <f ca="1">[1]Summary!$G35</f>
+        <f>[1]Summary!$G35</f>
         <v>874</v>
       </c>
       <c r="D32" t="s">
@@ -3946,7 +3946,7 @@
         <v>Certificate</v>
       </c>
       <c r="G32">
-        <f ca="1">[1]Summary!$H35</f>
+        <f>[1]Summary!$H35</f>
         <v>10875</v>
       </c>
       <c r="H32" t="s">
@@ -3969,7 +3969,7 @@
       </c>
       <c r="N32" t="str">
         <f t="shared" si="4"/>
-        <v>medical_administrative_assistant.pdf</v>
+        <v>medical_administrative_assistant_certificate.pdf</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -3978,11 +3978,11 @@
         <v>Medical Office Assistant Diploma</v>
       </c>
       <c r="B33" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>45.81818181818182</v>
       </c>
       <c r="C33" s="1">
-        <f ca="1">[1]Summary!$G36</f>
+        <f>[1]Summary!$G36</f>
         <v>1008</v>
       </c>
       <c r="D33" t="s">
@@ -3996,7 +3996,7 @@
         <v>Diploma</v>
       </c>
       <c r="G33">
-        <f ca="1">[1]Summary!$H36</f>
+        <f>[1]Summary!$H36</f>
         <v>14133</v>
       </c>
       <c r="H33" t="s">
@@ -4019,7 +4019,7 @@
       </c>
       <c r="N33" t="str">
         <f t="shared" si="4"/>
-        <v>medical_office_assistant.pdf</v>
+        <v>medical_office_assistant_diploma.pdf</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -4028,11 +4028,11 @@
         <v>Medical Office Assistant Diploma W/ Unit Clerk</v>
       </c>
       <c r="B34" s="1">
-        <f t="shared" ref="B34:B52" ca="1" si="5">C34/weeks</f>
+        <f t="shared" ref="B34:B52" si="5">C34/weeks</f>
         <v>59.18181818181818</v>
       </c>
       <c r="C34" s="1">
-        <f ca="1">[1]Summary!$G37</f>
+        <f>[1]Summary!$G37</f>
         <v>1302</v>
       </c>
       <c r="D34" t="s">
@@ -4046,7 +4046,7 @@
         <v>Diploma</v>
       </c>
       <c r="G34">
-        <f ca="1">[1]Summary!$H37</f>
+        <f>[1]Summary!$H37</f>
         <v>16455</v>
       </c>
       <c r="H34" t="s">
@@ -4069,7 +4069,7 @@
       </c>
       <c r="N34" t="str">
         <f t="shared" si="4"/>
-        <v>medical_office_assistant_w_unit_clerk.pdf</v>
+        <v>medical_office_assistant_w_unit_clerk_diploma.pdf</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -4078,11 +4078,11 @@
         <v>Medical Office Front Desk Assistant Certificate</v>
       </c>
       <c r="B35" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>26.09090909090909</v>
       </c>
       <c r="C35" s="1">
-        <f ca="1">[1]Summary!$G38</f>
+        <f>[1]Summary!$G38</f>
         <v>574</v>
       </c>
       <c r="D35" t="s">
@@ -4096,7 +4096,7 @@
         <v>Certificate</v>
       </c>
       <c r="G35">
-        <f ca="1">[1]Summary!$H38</f>
+        <f>[1]Summary!$H38</f>
         <v>7048</v>
       </c>
       <c r="H35" t="s">
@@ -4119,7 +4119,7 @@
       </c>
       <c r="N35" t="str">
         <f t="shared" si="4"/>
-        <v>medical_office_front_desk_assistant.pdf</v>
+        <v>medical_office_front_desk_assistant_certificate.pdf</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -4128,11 +4128,11 @@
         <v>Microsoft Certified Solutions Associate: Server Cert.</v>
       </c>
       <c r="B36" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>18.954545454545453</v>
       </c>
       <c r="C36" s="1">
-        <f ca="1">[1]Summary!$G39</f>
+        <f>[1]Summary!$G39</f>
         <v>417</v>
       </c>
       <c r="D36" t="s">
@@ -4146,7 +4146,7 @@
         <v>Certificate</v>
       </c>
       <c r="G36">
-        <f ca="1">[1]Summary!$H39</f>
+        <f>[1]Summary!$H39</f>
         <v>5624</v>
       </c>
       <c r="H36" t="s">
@@ -4169,7 +4169,7 @@
       </c>
       <c r="N36" t="str">
         <f t="shared" si="4"/>
-        <v>microsoft_certified_solutions_associate_server_cert_.pdf</v>
+        <v>microsoft_certified_solutions_associate_server_cert__certificate.pdf</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -4178,11 +4178,11 @@
         <v>Microsoft Certified Solutions Associate: Windows</v>
       </c>
       <c r="B37" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>18.954545454545453</v>
       </c>
       <c r="C37" s="1">
-        <f ca="1">[1]Summary!$G40</f>
+        <f>[1]Summary!$G40</f>
         <v>417</v>
       </c>
       <c r="D37" t="s">
@@ -4196,7 +4196,7 @@
         <v>Certificate</v>
       </c>
       <c r="G37">
-        <f ca="1">[1]Summary!$H40</f>
+        <f>[1]Summary!$H40</f>
         <v>5624</v>
       </c>
       <c r="H37" t="s">
@@ -4219,7 +4219,7 @@
       </c>
       <c r="N37" t="str">
         <f t="shared" si="4"/>
-        <v>microsoft_certified_solutions_associate_windows.pdf</v>
+        <v>microsoft_certified_solutions_associate_windows_certificate.pdf</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -4228,11 +4228,11 @@
         <v>Network Administrator Diploma (Server 2016)</v>
       </c>
       <c r="B38" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>79.681818181818187</v>
       </c>
       <c r="C38" s="1">
-        <f ca="1">[1]Summary!$G41</f>
+        <f>[1]Summary!$G41</f>
         <v>1753</v>
       </c>
       <c r="D38" t="s">
@@ -4246,7 +4246,7 @@
         <v>Diploma</v>
       </c>
       <c r="G38">
-        <f ca="1">[1]Summary!$H41</f>
+        <f>[1]Summary!$H41</f>
         <v>20916</v>
       </c>
       <c r="H38" t="s">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="N38" t="str">
         <f t="shared" si="4"/>
-        <v>network_administrator_server_2016.pdf</v>
+        <v>network_administrator_server_2016_diploma.pdf</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -4278,11 +4278,11 @@
         <v>Office Administration Assistant Certificate</v>
       </c>
       <c r="B39" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>21.454545454545453</v>
       </c>
       <c r="C39" s="1">
-        <f ca="1">[1]Summary!$G42</f>
+        <f>[1]Summary!$G42</f>
         <v>472</v>
       </c>
       <c r="D39" t="s">
@@ -4296,7 +4296,7 @@
         <v>Certificate</v>
       </c>
       <c r="G39">
-        <f ca="1">[1]Summary!$H42</f>
+        <f>[1]Summary!$H42</f>
         <v>6296</v>
       </c>
       <c r="H39" t="s">
@@ -4319,7 +4319,7 @@
       </c>
       <c r="N39" t="str">
         <f t="shared" si="4"/>
-        <v>office_administration_assistant.pdf</v>
+        <v>office_administration_assistant_certificate.pdf</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -4328,11 +4328,11 @@
         <v>Office Administration Diploma</v>
       </c>
       <c r="B40" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>48.227272727272727</v>
       </c>
       <c r="C40" s="1">
-        <f ca="1">[1]Summary!$G43</f>
+        <f>[1]Summary!$G43</f>
         <v>1061</v>
       </c>
       <c r="D40" t="s">
@@ -4346,7 +4346,7 @@
         <v>Diploma</v>
       </c>
       <c r="G40">
-        <f ca="1">[1]Summary!$H43</f>
+        <f>[1]Summary!$H43</f>
         <v>14251</v>
       </c>
       <c r="H40" t="s">
@@ -4369,7 +4369,7 @@
       </c>
       <c r="N40" t="str">
         <f t="shared" si="4"/>
-        <v>office_administration.pdf</v>
+        <v>office_administration_diploma.pdf</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -4378,11 +4378,11 @@
         <v>Office Clerk Certificate</v>
       </c>
       <c r="B41" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>19.772727272727273</v>
       </c>
       <c r="C41" s="1">
-        <f ca="1">[1]Summary!$G44</f>
+        <f>[1]Summary!$G44</f>
         <v>435</v>
       </c>
       <c r="D41" t="s">
@@ -4396,7 +4396,7 @@
         <v>Certificate</v>
       </c>
       <c r="G41">
-        <f ca="1">[1]Summary!$H44</f>
+        <f>[1]Summary!$H44</f>
         <v>5487</v>
       </c>
       <c r="H41" t="s">
@@ -4419,7 +4419,7 @@
       </c>
       <c r="N41" t="str">
         <f t="shared" si="4"/>
-        <v>office_clerk.pdf</v>
+        <v>office_clerk_certificate.pdf</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -4428,11 +4428,11 @@
         <v>Payroll Administrator Certificate</v>
       </c>
       <c r="B42" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>34.227272727272727</v>
       </c>
       <c r="C42" s="1">
-        <f ca="1">[1]Summary!$G45</f>
+        <f>[1]Summary!$G45</f>
         <v>753</v>
       </c>
       <c r="D42" t="s">
@@ -4446,7 +4446,7 @@
         <v>Certificate</v>
       </c>
       <c r="G42">
-        <f ca="1">[1]Summary!$H45</f>
+        <f>[1]Summary!$H45</f>
         <v>10882</v>
       </c>
       <c r="H42" t="s">
@@ -4469,7 +4469,7 @@
       </c>
       <c r="N42" t="str">
         <f t="shared" si="4"/>
-        <v>payroll_administrator.pdf</v>
+        <v>payroll_administrator_certificate.pdf</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -4478,11 +4478,11 @@
         <v>Payroll Clerk Certificate</v>
       </c>
       <c r="B43" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>24.454545454545453</v>
       </c>
       <c r="C43" s="1">
-        <f ca="1">[1]Summary!$G46</f>
+        <f>[1]Summary!$G46</f>
         <v>538</v>
       </c>
       <c r="D43" t="s">
@@ -4496,7 +4496,7 @@
         <v>Certificate</v>
       </c>
       <c r="G43">
-        <f ca="1">[1]Summary!$H46</f>
+        <f>[1]Summary!$H46</f>
         <v>7656</v>
       </c>
       <c r="H43" t="s">
@@ -4519,7 +4519,7 @@
       </c>
       <c r="N43" t="str">
         <f t="shared" si="4"/>
-        <v>payroll_clerk.pdf</v>
+        <v>payroll_clerk_certificate.pdf</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -4528,11 +4528,11 @@
         <v>Pc Support Specialist Diploma</v>
       </c>
       <c r="B44" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>52.909090909090907</v>
       </c>
       <c r="C44" s="1">
-        <f ca="1">[1]Summary!$G47</f>
+        <f>[1]Summary!$G47</f>
         <v>1164</v>
       </c>
       <c r="D44" t="s">
@@ -4546,7 +4546,7 @@
         <v>Diploma</v>
       </c>
       <c r="G44">
-        <f ca="1">[1]Summary!$H47</f>
+        <f>[1]Summary!$H47</f>
         <v>13604</v>
       </c>
       <c r="H44" t="s">
@@ -4569,7 +4569,7 @@
       </c>
       <c r="N44" t="str">
         <f t="shared" si="4"/>
-        <v>pc_support_specialist.pdf</v>
+        <v>pc_support_specialist_diploma.pdf</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -4578,11 +4578,11 @@
         <v>Project Administration Diploma</v>
       </c>
       <c r="B45" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>45.545454545454547</v>
       </c>
       <c r="C45" s="1">
-        <f ca="1">[1]Summary!$G48</f>
+        <f>[1]Summary!$G48</f>
         <v>1002</v>
       </c>
       <c r="D45" t="s">
@@ -4596,7 +4596,7 @@
         <v>Diploma</v>
       </c>
       <c r="G45">
-        <f ca="1">[1]Summary!$H48</f>
+        <f>[1]Summary!$H48</f>
         <v>14175</v>
       </c>
       <c r="H45" t="s">
@@ -4619,7 +4619,7 @@
       </c>
       <c r="N45" t="str">
         <f t="shared" si="4"/>
-        <v>project_administration.pdf</v>
+        <v>project_administration_diploma.pdf</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -4628,11 +4628,11 @@
         <v>Psa - Computerized Office Skills Certificate</v>
       </c>
       <c r="B46" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>10.545454545454545</v>
       </c>
       <c r="C46" s="1">
-        <f ca="1">[1]Summary!$G49</f>
+        <f>[1]Summary!$G49</f>
         <v>232</v>
       </c>
       <c r="D46" t="s">
@@ -4646,7 +4646,7 @@
         <v>Certificate</v>
       </c>
       <c r="G46">
-        <f ca="1">[1]Summary!$H49</f>
+        <f>[1]Summary!$H49</f>
         <v>3471</v>
       </c>
       <c r="H46" t="s">
@@ -4669,7 +4669,7 @@
       </c>
       <c r="N46" t="str">
         <f t="shared" si="4"/>
-        <v>psa_computerized_office_skills.pdf</v>
+        <v>psa_computerized_office_skills_certificate.pdf</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -4678,11 +4678,11 @@
         <v>Sales Associate Certificate</v>
       </c>
       <c r="B47" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>18.363636363636363</v>
       </c>
       <c r="C47" s="1">
-        <f ca="1">[1]Summary!$G50</f>
+        <f>[1]Summary!$G50</f>
         <v>404</v>
       </c>
       <c r="D47" t="s">
@@ -4696,7 +4696,7 @@
         <v>Certificate</v>
       </c>
       <c r="G47">
-        <f ca="1">[1]Summary!$H50</f>
+        <f>[1]Summary!$H50</f>
         <v>5651</v>
       </c>
       <c r="H47" t="s">
@@ -4719,7 +4719,7 @@
       </c>
       <c r="N47" t="str">
         <f t="shared" si="4"/>
-        <v>sales_associate.pdf</v>
+        <v>sales_associate_certificate.pdf</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -4728,11 +4728,11 @@
         <v>Sales Professional Diploma</v>
       </c>
       <c r="B48" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>38.363636363636367</v>
       </c>
       <c r="C48" s="1">
-        <f ca="1">[1]Summary!$G51</f>
+        <f>[1]Summary!$G51</f>
         <v>844</v>
       </c>
       <c r="D48" t="s">
@@ -4746,7 +4746,7 @@
         <v>Diploma</v>
       </c>
       <c r="G48">
-        <f ca="1">[1]Summary!$H51</f>
+        <f>[1]Summary!$H51</f>
         <v>11787</v>
       </c>
       <c r="H48" t="s">
@@ -4769,7 +4769,7 @@
       </c>
       <c r="N48" t="str">
         <f t="shared" si="4"/>
-        <v>sales_professional.pdf</v>
+        <v>sales_professional_diploma.pdf</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
@@ -4778,11 +4778,11 @@
         <v>Software And Web Developer Diploma</v>
       </c>
       <c r="B49" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>43.136363636363633</v>
       </c>
       <c r="C49" s="1">
-        <f ca="1">[1]Summary!$G52</f>
+        <f>[1]Summary!$G52</f>
         <v>949</v>
       </c>
       <c r="D49" t="s">
@@ -4796,7 +4796,7 @@
         <v>Diploma</v>
       </c>
       <c r="G49">
-        <f ca="1">[1]Summary!$H52</f>
+        <f>[1]Summary!$H52</f>
         <v>17063</v>
       </c>
       <c r="H49" t="s">
@@ -4819,7 +4819,7 @@
       </c>
       <c r="N49" t="str">
         <f t="shared" si="4"/>
-        <v>software_and_web_developer.pdf</v>
+        <v>software_and_web_developer_diploma.pdf</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -4828,11 +4828,11 @@
         <v>Web Designer Diploma</v>
       </c>
       <c r="B50" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>53.772727272727273</v>
       </c>
       <c r="C50" s="1">
-        <f ca="1">[1]Summary!$G53</f>
+        <f>[1]Summary!$G53</f>
         <v>1183</v>
       </c>
       <c r="D50" t="s">
@@ -4846,7 +4846,7 @@
         <v>Diploma</v>
       </c>
       <c r="G50">
-        <f ca="1">[1]Summary!$H53</f>
+        <f>[1]Summary!$H53</f>
         <v>17114</v>
       </c>
       <c r="H50" t="s">
@@ -4869,7 +4869,7 @@
       </c>
       <c r="N50" t="str">
         <f t="shared" si="4"/>
-        <v>web_designer.pdf</v>
+        <v>web_designer_diploma.pdf</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
@@ -4878,11 +4878,11 @@
         <v>Web Developer Diploma</v>
       </c>
       <c r="B51" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>26.863636363636363</v>
       </c>
       <c r="C51" s="1">
-        <f ca="1">[1]Summary!$G54</f>
+        <f>[1]Summary!$G54</f>
         <v>591</v>
       </c>
       <c r="D51" t="s">
@@ -4896,7 +4896,7 @@
         <v>Diploma</v>
       </c>
       <c r="G51">
-        <f ca="1">[1]Summary!$H54</f>
+        <f>[1]Summary!$H54</f>
         <v>10774</v>
       </c>
       <c r="H51" t="s">
@@ -4919,7 +4919,7 @@
       </c>
       <c r="N51" t="str">
         <f t="shared" si="4"/>
-        <v>web_developer.pdf</v>
+        <v>web_developer_diploma.pdf</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
@@ -4964,8 +4964,8 @@
         <v>it_tech_support_specialist_programdata.json</v>
       </c>
       <c r="N52" t="str">
-        <f t="shared" ref="N52" si="9">_xlfn.CONCAT(L52,".pdf")</f>
-        <v>it_tech_support_specialist.pdf</v>
+        <f t="shared" si="4"/>
+        <v>it_tech_support_specialist_diploma.pdf</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix hours for business admin
</commit_message>
<xml_diff>
--- a/static/programlisting.xlsx
+++ b/static/programlisting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\aolccbc.com\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB5BD0C-7930-4645-AFF4-7DA68E7C425D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1E604E-3D1E-41EC-9337-BFDE1F1E56BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -722,59 +722,59 @@
       <sheetName val="Reference"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
+      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="49" refreshError="1"/>
+      <sheetData sheetId="50" refreshError="1"/>
+      <sheetData sheetId="51" refreshError="1"/>
+      <sheetData sheetId="52" refreshError="1"/>
       <sheetData sheetId="53">
         <row r="5">
           <cell r="A5" t="str">
@@ -869,7 +869,7 @@
             <v>BUSINESS ADMINISTRATION CO-OP DIPLOMA</v>
           </cell>
           <cell r="G13">
-            <v>141</v>
+            <v>2137</v>
           </cell>
           <cell r="H13">
             <v>22293</v>
@@ -880,7 +880,7 @@
             <v>BUSINESS ADMINISTRATION DIPLOMA</v>
           </cell>
           <cell r="G14">
-            <v>136</v>
+            <v>1267</v>
           </cell>
           <cell r="H14">
             <v>17893</v>
@@ -2047,8 +2047,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
+      <sheetData sheetId="55" refreshError="1"/>
+      <sheetData sheetId="56" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2353,8 +2353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2419,11 +2419,11 @@
         <v>A+ Network+ And Mcsa Desktop Cert. Prep</v>
       </c>
       <c r="B2" s="1">
-        <f t="shared" ref="B2:B33" si="0">C2/weeks</f>
+        <f t="shared" ref="B2:B33" ca="1" si="0">C2/weeks</f>
         <v>34.090909090909093</v>
       </c>
       <c r="C2" s="1">
-        <f>[1]Summary!$G5</f>
+        <f ca="1">[1]Summary!$G5</f>
         <v>750</v>
       </c>
       <c r="D2" t="s">
@@ -2437,7 +2437,7 @@
         <v>Certificate</v>
       </c>
       <c r="G2">
-        <f>[1]Summary!$H5</f>
+        <f ca="1">[1]Summary!$H5</f>
         <v>8510</v>
       </c>
       <c r="H2" t="s">
@@ -2469,11 +2469,11 @@
         <v>Accounting Administrator Diploma With Sage</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>35.863636363636367</v>
       </c>
       <c r="C3" s="1">
-        <f>[1]Summary!$G6</f>
+        <f ca="1">[1]Summary!$G6</f>
         <v>789</v>
       </c>
       <c r="D3" t="s">
@@ -2487,7 +2487,7 @@
         <v>Diploma</v>
       </c>
       <c r="G3">
-        <f>[1]Summary!$H6</f>
+        <f ca="1">[1]Summary!$H6</f>
         <v>11559</v>
       </c>
       <c r="H3" t="s">
@@ -2519,11 +2519,11 @@
         <v>Accounting And Business Technology Diploma</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>40.863636363636367</v>
       </c>
       <c r="C4" s="1">
-        <f>[1]Summary!$G7</f>
+        <f ca="1">[1]Summary!$G7</f>
         <v>899</v>
       </c>
       <c r="D4" t="s">
@@ -2537,7 +2537,7 @@
         <v>Diploma</v>
       </c>
       <c r="G4">
-        <f>[1]Summary!$H7</f>
+        <f ca="1">[1]Summary!$H7</f>
         <v>12729</v>
       </c>
       <c r="H4" t="s">
@@ -2569,11 +2569,11 @@
         <v>Accounting And Payroll Administrator Diploma</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>49.272727272727273</v>
       </c>
       <c r="C5" s="1">
-        <f>[1]Summary!$G8</f>
+        <f ca="1">[1]Summary!$G8</f>
         <v>1084</v>
       </c>
       <c r="D5" t="s">
@@ -2587,7 +2587,7 @@
         <v>Diploma</v>
       </c>
       <c r="G5">
-        <f>[1]Summary!$H8</f>
+        <f ca="1">[1]Summary!$H8</f>
         <v>15180</v>
       </c>
       <c r="H5" t="s">
@@ -2619,11 +2619,11 @@
         <v>Accounting Bookkeeper Certificate</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>29.227272727272727</v>
       </c>
       <c r="C6" s="1">
-        <f>[1]Summary!$G9</f>
+        <f ca="1">[1]Summary!$G9</f>
         <v>643</v>
       </c>
       <c r="D6" t="s">
@@ -2637,7 +2637,7 @@
         <v>Certificate</v>
       </c>
       <c r="G6">
-        <f>[1]Summary!$H9</f>
+        <f ca="1">[1]Summary!$H9</f>
         <v>8707</v>
       </c>
       <c r="H6" t="s">
@@ -2669,11 +2669,11 @@
         <v>Accounting Clerk Certificate</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>20.90909090909091</v>
       </c>
       <c r="C7" s="1">
-        <f>[1]Summary!$G10</f>
+        <f ca="1">[1]Summary!$G10</f>
         <v>460</v>
       </c>
       <c r="D7" t="s">
@@ -2687,7 +2687,7 @@
         <v>Certificate</v>
       </c>
       <c r="G7">
-        <f>[1]Summary!$H10</f>
+        <f ca="1">[1]Summary!$H10</f>
         <v>6452</v>
       </c>
       <c r="H7" t="s">
@@ -2719,11 +2719,11 @@
         <v>Addictions Worker Certificate</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>13.636363636363637</v>
       </c>
       <c r="C8" s="1">
-        <f>[1]Summary!$G11</f>
+        <f ca="1">[1]Summary!$G11</f>
         <v>300</v>
       </c>
       <c r="D8" t="s">
@@ -2737,7 +2737,7 @@
         <v>Certificate</v>
       </c>
       <c r="G8">
-        <f>[1]Summary!$H11</f>
+        <f ca="1">[1]Summary!$H11</f>
         <v>3079</v>
       </c>
       <c r="H8" t="s">
@@ -2769,11 +2769,11 @@
         <v>Administrative Assistant Diploma</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>34.909090909090907</v>
       </c>
       <c r="C9" s="1">
-        <f>[1]Summary!$G12</f>
+        <f ca="1">[1]Summary!$G12</f>
         <v>768</v>
       </c>
       <c r="D9" t="s">
@@ -2787,7 +2787,7 @@
         <v>Diploma</v>
       </c>
       <c r="G9">
-        <f>[1]Summary!$H12</f>
+        <f ca="1">[1]Summary!$H12</f>
         <v>10097</v>
       </c>
       <c r="H9" t="s">
@@ -2819,12 +2819,12 @@
         <v>Business Administration Co-Op Diploma</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="0"/>
-        <v>6.4090909090909092</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>97.13636363636364</v>
       </c>
       <c r="C10" s="1">
-        <f>[1]Summary!$G13</f>
-        <v>141</v>
+        <f ca="1">[1]Summary!$G13</f>
+        <v>2137</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -2837,7 +2837,7 @@
         <v>Diploma</v>
       </c>
       <c r="G10">
-        <f>[1]Summary!$H13</f>
+        <f ca="1">[1]Summary!$H13</f>
         <v>22293</v>
       </c>
       <c r="H10" t="s">
@@ -2869,12 +2869,12 @@
         <v>Business Administration Diploma</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="0"/>
-        <v>6.1818181818181817</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>57.590909090909093</v>
       </c>
       <c r="C11" s="1">
-        <f>[1]Summary!$G14</f>
-        <v>136</v>
+        <f ca="1">[1]Summary!$G14</f>
+        <v>1267</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -2887,7 +2887,7 @@
         <v>Diploma</v>
       </c>
       <c r="G11">
-        <f>[1]Summary!$H14</f>
+        <f ca="1">[1]Summary!$H14</f>
         <v>17893</v>
       </c>
       <c r="H11" t="s">
@@ -2919,11 +2919,11 @@
         <v>Business Management Certificate</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>28.045454545454547</v>
       </c>
       <c r="C12" s="1">
-        <f>[1]Summary!$G15</f>
+        <f ca="1">[1]Summary!$G15</f>
         <v>617</v>
       </c>
       <c r="D12" t="s">
@@ -2937,7 +2937,7 @@
         <v>Certificate</v>
       </c>
       <c r="G12">
-        <f>[1]Summary!$H15</f>
+        <f ca="1">[1]Summary!$H15</f>
         <v>9329</v>
       </c>
       <c r="H12" t="s">
@@ -2969,11 +2969,11 @@
         <v>Business Office Skills Diploma</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>38.31818181818182</v>
       </c>
       <c r="C13" s="1">
-        <f>[1]Summary!$G16</f>
+        <f ca="1">[1]Summary!$G16</f>
         <v>843</v>
       </c>
       <c r="D13" t="s">
@@ -2987,7 +2987,7 @@
         <v>Diploma</v>
       </c>
       <c r="G13">
-        <f>[1]Summary!$H16</f>
+        <f ca="1">[1]Summary!$H16</f>
         <v>11409</v>
       </c>
       <c r="H13" t="s">
@@ -3019,11 +3019,11 @@
         <v>Business Receptionist Certificate</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>24.59090909090909</v>
       </c>
       <c r="C14" s="1">
-        <f>[1]Summary!$G17</f>
+        <f ca="1">[1]Summary!$G17</f>
         <v>541</v>
       </c>
       <c r="D14" t="s">
@@ -3037,7 +3037,7 @@
         <v>Certificate</v>
       </c>
       <c r="G14">
-        <f>[1]Summary!$H17</f>
+        <f ca="1">[1]Summary!$H17</f>
         <v>7135</v>
       </c>
       <c r="H14" t="s">
@@ -3069,11 +3069,11 @@
         <v>Business Service Essentials Co-Op Diploma</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>48.909090909090907</v>
       </c>
       <c r="C15" s="1">
-        <f>[1]Summary!$G18</f>
+        <f ca="1">[1]Summary!$G18</f>
         <v>1076</v>
       </c>
       <c r="D15" t="s">
@@ -3087,7 +3087,7 @@
         <v>Diploma</v>
       </c>
       <c r="G15">
-        <f>[1]Summary!$H18</f>
+        <f ca="1">[1]Summary!$H18</f>
         <v>10752</v>
       </c>
       <c r="H15" t="s">
@@ -3119,11 +3119,11 @@
         <v>Call Centre Customer Representative Diploma</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>31.181818181818183</v>
       </c>
       <c r="C16" s="1">
-        <f>[1]Summary!$G19</f>
+        <f ca="1">[1]Summary!$G19</f>
         <v>686</v>
       </c>
       <c r="D16" t="s">
@@ -3137,7 +3137,7 @@
         <v>Diploma</v>
       </c>
       <c r="G16">
-        <f>[1]Summary!$H19</f>
+        <f ca="1">[1]Summary!$H19</f>
         <v>9627</v>
       </c>
       <c r="H16" t="s">
@@ -3169,11 +3169,11 @@
         <v>Community Service Worker And Addictions Worker Diploma</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>52.590909090909093</v>
       </c>
       <c r="C17" s="1">
-        <f>[1]Summary!$G20</f>
+        <f ca="1">[1]Summary!$G20</f>
         <v>1157</v>
       </c>
       <c r="D17" t="s">
@@ -3187,7 +3187,7 @@
         <v>Diploma</v>
       </c>
       <c r="G17">
-        <f>[1]Summary!$H20</f>
+        <f ca="1">[1]Summary!$H20</f>
         <v>15449</v>
       </c>
       <c r="H17" t="s">
@@ -3219,11 +3219,11 @@
         <v>Community Service Worker Diploma</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>37.590909090909093</v>
       </c>
       <c r="C18" s="1">
-        <f>[1]Summary!$G21</f>
+        <f ca="1">[1]Summary!$G21</f>
         <v>827</v>
       </c>
       <c r="D18" t="s">
@@ -3237,7 +3237,7 @@
         <v>Diploma</v>
       </c>
       <c r="G18">
-        <f>[1]Summary!$H21</f>
+        <f ca="1">[1]Summary!$H21</f>
         <v>12370</v>
       </c>
       <c r="H18" t="s">
@@ -3272,11 +3272,11 @@
         <v>Computer Service Technician Certificate</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>26.636363636363637</v>
       </c>
       <c r="C19" s="1">
-        <f>[1]Summary!$G22</f>
+        <f ca="1">[1]Summary!$G22</f>
         <v>586</v>
       </c>
       <c r="D19" t="s">
@@ -3290,7 +3290,7 @@
         <v>Certificate</v>
       </c>
       <c r="G19">
-        <f>[1]Summary!$H22</f>
+        <f ca="1">[1]Summary!$H22</f>
         <v>5822</v>
       </c>
       <c r="H19" t="s">
@@ -3325,11 +3325,11 @@
         <v>Computer Service Technician Diploma</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>46.31818181818182</v>
       </c>
       <c r="C20" s="1">
-        <f>[1]Summary!$G23</f>
+        <f ca="1">[1]Summary!$G23</f>
         <v>1019</v>
       </c>
       <c r="D20" t="s">
@@ -3343,7 +3343,7 @@
         <v>Diploma</v>
       </c>
       <c r="G20">
-        <f>[1]Summary!$H23</f>
+        <f ca="1">[1]Summary!$H23</f>
         <v>12167</v>
       </c>
       <c r="H20" t="s">
@@ -3378,11 +3378,11 @@
         <v>Computer Software Support Diploma</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>46.31818181818182</v>
       </c>
       <c r="C21" s="1">
-        <f>[1]Summary!$G24</f>
+        <f ca="1">[1]Summary!$G24</f>
         <v>1019</v>
       </c>
       <c r="D21" t="s">
@@ -3396,7 +3396,7 @@
         <v>Diploma</v>
       </c>
       <c r="G21">
-        <f>[1]Summary!$H24</f>
+        <f ca="1">[1]Summary!$H24</f>
         <v>12167</v>
       </c>
       <c r="H21" t="s">
@@ -3428,11 +3428,11 @@
         <v>Computerized Office Procedures Certificate</v>
       </c>
       <c r="B22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>25.59090909090909</v>
       </c>
       <c r="C22" s="1">
-        <f>[1]Summary!$G25</f>
+        <f ca="1">[1]Summary!$G25</f>
         <v>563</v>
       </c>
       <c r="D22" t="s">
@@ -3446,7 +3446,7 @@
         <v>Certificate</v>
       </c>
       <c r="G22">
-        <f>[1]Summary!$H25</f>
+        <f ca="1">[1]Summary!$H25</f>
         <v>7132</v>
       </c>
       <c r="H22" t="s">
@@ -3478,11 +3478,11 @@
         <v>Conference And Event Planner Diploma</v>
       </c>
       <c r="B23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>46.227272727272727</v>
       </c>
       <c r="C23" s="1">
-        <f>[1]Summary!$G26</f>
+        <f ca="1">[1]Summary!$G26</f>
         <v>1017</v>
       </c>
       <c r="D23" t="s">
@@ -3496,7 +3496,7 @@
         <v>Diploma</v>
       </c>
       <c r="G23">
-        <f>[1]Summary!$H26</f>
+        <f ca="1">[1]Summary!$H26</f>
         <v>14474</v>
       </c>
       <c r="H23" t="s">
@@ -3528,11 +3528,11 @@
         <v>Customer Service Representative Certificate</v>
       </c>
       <c r="B24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>20.727272727272727</v>
       </c>
       <c r="C24" s="1">
-        <f>[1]Summary!$G27</f>
+        <f ca="1">[1]Summary!$G27</f>
         <v>456</v>
       </c>
       <c r="D24" t="s">
@@ -3546,7 +3546,7 @@
         <v>Certificate</v>
       </c>
       <c r="G24">
-        <f>[1]Summary!$H27</f>
+        <f ca="1">[1]Summary!$H27</f>
         <v>6271</v>
       </c>
       <c r="H24" t="s">
@@ -3578,11 +3578,11 @@
         <v>English As Second Language</v>
       </c>
       <c r="B25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>14.545454545454545</v>
       </c>
       <c r="C25" s="1">
-        <f>[1]Summary!$G28</f>
+        <f ca="1">[1]Summary!$G28</f>
         <v>320</v>
       </c>
       <c r="D25" t="s">
@@ -3596,7 +3596,7 @@
         <v>Certificate</v>
       </c>
       <c r="G25">
-        <f>[1]Summary!$H28</f>
+        <f ca="1">[1]Summary!$H28</f>
         <v>3390</v>
       </c>
       <c r="H25" t="s">
@@ -3628,11 +3628,11 @@
         <v>Entrepreneurial Business Applications Diploma</v>
       </c>
       <c r="B26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>41.18181818181818</v>
       </c>
       <c r="C26" s="1">
-        <f>[1]Summary!$G29</f>
+        <f ca="1">[1]Summary!$G29</f>
         <v>906</v>
       </c>
       <c r="D26" t="s">
@@ -3646,7 +3646,7 @@
         <v>Diploma</v>
       </c>
       <c r="G26">
-        <f>[1]Summary!$H29</f>
+        <f ca="1">[1]Summary!$H29</f>
         <v>12541</v>
       </c>
       <c r="H26" t="s">
@@ -3678,11 +3678,11 @@
         <v>Executive Assistant Diploma</v>
       </c>
       <c r="B27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>48.136363636363633</v>
       </c>
       <c r="C27" s="1">
-        <f>[1]Summary!$G30</f>
+        <f ca="1">[1]Summary!$G30</f>
         <v>1059</v>
       </c>
       <c r="D27" t="s">
@@ -3696,7 +3696,7 @@
         <v>Diploma</v>
       </c>
       <c r="G27">
-        <f>[1]Summary!$H30</f>
+        <f ca="1">[1]Summary!$H30</f>
         <v>14334</v>
       </c>
       <c r="H27" t="s">
@@ -3728,11 +3728,11 @@
         <v>Graphic Designer Diploma</v>
       </c>
       <c r="B28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>49.454545454545453</v>
       </c>
       <c r="C28" s="1">
-        <f>[1]Summary!$G31</f>
+        <f ca="1">[1]Summary!$G31</f>
         <v>1088</v>
       </c>
       <c r="D28" t="s">
@@ -3746,7 +3746,7 @@
         <v>Diploma</v>
       </c>
       <c r="G28">
-        <f>[1]Summary!$H31</f>
+        <f ca="1">[1]Summary!$H31</f>
         <v>16396</v>
       </c>
       <c r="H28" t="s">
@@ -3778,11 +3778,11 @@
         <v>Human Resources Administration Certificate</v>
       </c>
       <c r="B29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>29.09090909090909</v>
       </c>
       <c r="C29" s="1">
-        <f>[1]Summary!$G32</f>
+        <f ca="1">[1]Summary!$G32</f>
         <v>640</v>
       </c>
       <c r="D29" t="s">
@@ -3796,7 +3796,7 @@
         <v>Certificate</v>
       </c>
       <c r="G29">
-        <f>[1]Summary!$H32</f>
+        <f ca="1">[1]Summary!$H32</f>
         <v>8468</v>
       </c>
       <c r="H29" t="s">
@@ -3828,11 +3828,11 @@
         <v>Marketing Administrative Assistant Certificate</v>
       </c>
       <c r="B30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>34.545454545454547</v>
       </c>
       <c r="C30" s="1">
-        <f>[1]Summary!$G33</f>
+        <f ca="1">[1]Summary!$G33</f>
         <v>760</v>
       </c>
       <c r="D30" t="s">
@@ -3846,7 +3846,7 @@
         <v>Certificate</v>
       </c>
       <c r="G30">
-        <f>[1]Summary!$H33</f>
+        <f ca="1">[1]Summary!$H33</f>
         <v>10655</v>
       </c>
       <c r="H30" t="s">
@@ -3878,11 +3878,11 @@
         <v>Marketing Coordinator Diploma</v>
       </c>
       <c r="B31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>43.045454545454547</v>
       </c>
       <c r="C31" s="1">
-        <f>[1]Summary!$G34</f>
+        <f ca="1">[1]Summary!$G34</f>
         <v>947</v>
       </c>
       <c r="D31" t="s">
@@ -3896,7 +3896,7 @@
         <v>Diploma</v>
       </c>
       <c r="G31">
-        <f>[1]Summary!$H34</f>
+        <f ca="1">[1]Summary!$H34</f>
         <v>14242</v>
       </c>
       <c r="H31" t="s">
@@ -3928,11 +3928,11 @@
         <v>Medical Administrative Assistant Certificate</v>
       </c>
       <c r="B32" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>39.727272727272727</v>
       </c>
       <c r="C32" s="1">
-        <f>[1]Summary!$G35</f>
+        <f ca="1">[1]Summary!$G35</f>
         <v>874</v>
       </c>
       <c r="D32" t="s">
@@ -3946,7 +3946,7 @@
         <v>Certificate</v>
       </c>
       <c r="G32">
-        <f>[1]Summary!$H35</f>
+        <f ca="1">[1]Summary!$H35</f>
         <v>10875</v>
       </c>
       <c r="H32" t="s">
@@ -3978,11 +3978,11 @@
         <v>Medical Office Assistant Diploma</v>
       </c>
       <c r="B33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>45.81818181818182</v>
       </c>
       <c r="C33" s="1">
-        <f>[1]Summary!$G36</f>
+        <f ca="1">[1]Summary!$G36</f>
         <v>1008</v>
       </c>
       <c r="D33" t="s">
@@ -3996,7 +3996,7 @@
         <v>Diploma</v>
       </c>
       <c r="G33">
-        <f>[1]Summary!$H36</f>
+        <f ca="1">[1]Summary!$H36</f>
         <v>14133</v>
       </c>
       <c r="H33" t="s">
@@ -4028,11 +4028,11 @@
         <v>Medical Office Assistant Diploma W/ Unit Clerk</v>
       </c>
       <c r="B34" s="1">
-        <f t="shared" ref="B34:B52" si="5">C34/weeks</f>
+        <f t="shared" ref="B34:B52" ca="1" si="5">C34/weeks</f>
         <v>59.18181818181818</v>
       </c>
       <c r="C34" s="1">
-        <f>[1]Summary!$G37</f>
+        <f ca="1">[1]Summary!$G37</f>
         <v>1302</v>
       </c>
       <c r="D34" t="s">
@@ -4046,7 +4046,7 @@
         <v>Diploma</v>
       </c>
       <c r="G34">
-        <f>[1]Summary!$H37</f>
+        <f ca="1">[1]Summary!$H37</f>
         <v>16455</v>
       </c>
       <c r="H34" t="s">
@@ -4078,11 +4078,11 @@
         <v>Medical Office Front Desk Assistant Certificate</v>
       </c>
       <c r="B35" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>26.09090909090909</v>
       </c>
       <c r="C35" s="1">
-        <f>[1]Summary!$G38</f>
+        <f ca="1">[1]Summary!$G38</f>
         <v>574</v>
       </c>
       <c r="D35" t="s">
@@ -4096,7 +4096,7 @@
         <v>Certificate</v>
       </c>
       <c r="G35">
-        <f>[1]Summary!$H38</f>
+        <f ca="1">[1]Summary!$H38</f>
         <v>7048</v>
       </c>
       <c r="H35" t="s">
@@ -4128,11 +4128,11 @@
         <v>Microsoft Certified Solutions Associate: Server Cert.</v>
       </c>
       <c r="B36" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>18.954545454545453</v>
       </c>
       <c r="C36" s="1">
-        <f>[1]Summary!$G39</f>
+        <f ca="1">[1]Summary!$G39</f>
         <v>417</v>
       </c>
       <c r="D36" t="s">
@@ -4146,7 +4146,7 @@
         <v>Certificate</v>
       </c>
       <c r="G36">
-        <f>[1]Summary!$H39</f>
+        <f ca="1">[1]Summary!$H39</f>
         <v>5624</v>
       </c>
       <c r="H36" t="s">
@@ -4178,11 +4178,11 @@
         <v>Microsoft Certified Solutions Associate: Windows</v>
       </c>
       <c r="B37" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>18.954545454545453</v>
       </c>
       <c r="C37" s="1">
-        <f>[1]Summary!$G40</f>
+        <f ca="1">[1]Summary!$G40</f>
         <v>417</v>
       </c>
       <c r="D37" t="s">
@@ -4196,7 +4196,7 @@
         <v>Certificate</v>
       </c>
       <c r="G37">
-        <f>[1]Summary!$H40</f>
+        <f ca="1">[1]Summary!$H40</f>
         <v>5624</v>
       </c>
       <c r="H37" t="s">
@@ -4228,11 +4228,11 @@
         <v>Network Administrator Diploma (Server 2016)</v>
       </c>
       <c r="B38" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>79.681818181818187</v>
       </c>
       <c r="C38" s="1">
-        <f>[1]Summary!$G41</f>
+        <f ca="1">[1]Summary!$G41</f>
         <v>1753</v>
       </c>
       <c r="D38" t="s">
@@ -4246,7 +4246,7 @@
         <v>Diploma</v>
       </c>
       <c r="G38">
-        <f>[1]Summary!$H41</f>
+        <f ca="1">[1]Summary!$H41</f>
         <v>20916</v>
       </c>
       <c r="H38" t="s">
@@ -4278,11 +4278,11 @@
         <v>Office Administration Assistant Certificate</v>
       </c>
       <c r="B39" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>21.454545454545453</v>
       </c>
       <c r="C39" s="1">
-        <f>[1]Summary!$G42</f>
+        <f ca="1">[1]Summary!$G42</f>
         <v>472</v>
       </c>
       <c r="D39" t="s">
@@ -4296,7 +4296,7 @@
         <v>Certificate</v>
       </c>
       <c r="G39">
-        <f>[1]Summary!$H42</f>
+        <f ca="1">[1]Summary!$H42</f>
         <v>6296</v>
       </c>
       <c r="H39" t="s">
@@ -4328,11 +4328,11 @@
         <v>Office Administration Diploma</v>
       </c>
       <c r="B40" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>48.227272727272727</v>
       </c>
       <c r="C40" s="1">
-        <f>[1]Summary!$G43</f>
+        <f ca="1">[1]Summary!$G43</f>
         <v>1061</v>
       </c>
       <c r="D40" t="s">
@@ -4346,7 +4346,7 @@
         <v>Diploma</v>
       </c>
       <c r="G40">
-        <f>[1]Summary!$H43</f>
+        <f ca="1">[1]Summary!$H43</f>
         <v>14251</v>
       </c>
       <c r="H40" t="s">
@@ -4378,11 +4378,11 @@
         <v>Office Clerk Certificate</v>
       </c>
       <c r="B41" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>19.772727272727273</v>
       </c>
       <c r="C41" s="1">
-        <f>[1]Summary!$G44</f>
+        <f ca="1">[1]Summary!$G44</f>
         <v>435</v>
       </c>
       <c r="D41" t="s">
@@ -4396,7 +4396,7 @@
         <v>Certificate</v>
       </c>
       <c r="G41">
-        <f>[1]Summary!$H44</f>
+        <f ca="1">[1]Summary!$H44</f>
         <v>5487</v>
       </c>
       <c r="H41" t="s">
@@ -4428,11 +4428,11 @@
         <v>Payroll Administrator Certificate</v>
       </c>
       <c r="B42" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>34.227272727272727</v>
       </c>
       <c r="C42" s="1">
-        <f>[1]Summary!$G45</f>
+        <f ca="1">[1]Summary!$G45</f>
         <v>753</v>
       </c>
       <c r="D42" t="s">
@@ -4446,7 +4446,7 @@
         <v>Certificate</v>
       </c>
       <c r="G42">
-        <f>[1]Summary!$H45</f>
+        <f ca="1">[1]Summary!$H45</f>
         <v>10882</v>
       </c>
       <c r="H42" t="s">
@@ -4478,11 +4478,11 @@
         <v>Payroll Clerk Certificate</v>
       </c>
       <c r="B43" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>24.454545454545453</v>
       </c>
       <c r="C43" s="1">
-        <f>[1]Summary!$G46</f>
+        <f ca="1">[1]Summary!$G46</f>
         <v>538</v>
       </c>
       <c r="D43" t="s">
@@ -4496,7 +4496,7 @@
         <v>Certificate</v>
       </c>
       <c r="G43">
-        <f>[1]Summary!$H46</f>
+        <f ca="1">[1]Summary!$H46</f>
         <v>7656</v>
       </c>
       <c r="H43" t="s">
@@ -4528,11 +4528,11 @@
         <v>Pc Support Specialist Diploma</v>
       </c>
       <c r="B44" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>52.909090909090907</v>
       </c>
       <c r="C44" s="1">
-        <f>[1]Summary!$G47</f>
+        <f ca="1">[1]Summary!$G47</f>
         <v>1164</v>
       </c>
       <c r="D44" t="s">
@@ -4546,7 +4546,7 @@
         <v>Diploma</v>
       </c>
       <c r="G44">
-        <f>[1]Summary!$H47</f>
+        <f ca="1">[1]Summary!$H47</f>
         <v>13604</v>
       </c>
       <c r="H44" t="s">
@@ -4578,11 +4578,11 @@
         <v>Project Administration Diploma</v>
       </c>
       <c r="B45" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>45.545454545454547</v>
       </c>
       <c r="C45" s="1">
-        <f>[1]Summary!$G48</f>
+        <f ca="1">[1]Summary!$G48</f>
         <v>1002</v>
       </c>
       <c r="D45" t="s">
@@ -4596,7 +4596,7 @@
         <v>Diploma</v>
       </c>
       <c r="G45">
-        <f>[1]Summary!$H48</f>
+        <f ca="1">[1]Summary!$H48</f>
         <v>14175</v>
       </c>
       <c r="H45" t="s">
@@ -4628,11 +4628,11 @@
         <v>Psa - Computerized Office Skills Certificate</v>
       </c>
       <c r="B46" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.545454545454545</v>
       </c>
       <c r="C46" s="1">
-        <f>[1]Summary!$G49</f>
+        <f ca="1">[1]Summary!$G49</f>
         <v>232</v>
       </c>
       <c r="D46" t="s">
@@ -4646,7 +4646,7 @@
         <v>Certificate</v>
       </c>
       <c r="G46">
-        <f>[1]Summary!$H49</f>
+        <f ca="1">[1]Summary!$H49</f>
         <v>3471</v>
       </c>
       <c r="H46" t="s">
@@ -4678,11 +4678,11 @@
         <v>Sales Associate Certificate</v>
       </c>
       <c r="B47" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>18.363636363636363</v>
       </c>
       <c r="C47" s="1">
-        <f>[1]Summary!$G50</f>
+        <f ca="1">[1]Summary!$G50</f>
         <v>404</v>
       </c>
       <c r="D47" t="s">
@@ -4696,7 +4696,7 @@
         <v>Certificate</v>
       </c>
       <c r="G47">
-        <f>[1]Summary!$H50</f>
+        <f ca="1">[1]Summary!$H50</f>
         <v>5651</v>
       </c>
       <c r="H47" t="s">
@@ -4728,11 +4728,11 @@
         <v>Sales Professional Diploma</v>
       </c>
       <c r="B48" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>38.363636363636367</v>
       </c>
       <c r="C48" s="1">
-        <f>[1]Summary!$G51</f>
+        <f ca="1">[1]Summary!$G51</f>
         <v>844</v>
       </c>
       <c r="D48" t="s">
@@ -4746,7 +4746,7 @@
         <v>Diploma</v>
       </c>
       <c r="G48">
-        <f>[1]Summary!$H51</f>
+        <f ca="1">[1]Summary!$H51</f>
         <v>11787</v>
       </c>
       <c r="H48" t="s">
@@ -4778,11 +4778,11 @@
         <v>Software And Web Developer Diploma</v>
       </c>
       <c r="B49" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>43.136363636363633</v>
       </c>
       <c r="C49" s="1">
-        <f>[1]Summary!$G52</f>
+        <f ca="1">[1]Summary!$G52</f>
         <v>949</v>
       </c>
       <c r="D49" t="s">
@@ -4796,7 +4796,7 @@
         <v>Diploma</v>
       </c>
       <c r="G49">
-        <f>[1]Summary!$H52</f>
+        <f ca="1">[1]Summary!$H52</f>
         <v>17063</v>
       </c>
       <c r="H49" t="s">
@@ -4828,11 +4828,11 @@
         <v>Web Designer Diploma</v>
       </c>
       <c r="B50" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>53.772727272727273</v>
       </c>
       <c r="C50" s="1">
-        <f>[1]Summary!$G53</f>
+        <f ca="1">[1]Summary!$G53</f>
         <v>1183</v>
       </c>
       <c r="D50" t="s">
@@ -4846,7 +4846,7 @@
         <v>Diploma</v>
       </c>
       <c r="G50">
-        <f>[1]Summary!$H53</f>
+        <f ca="1">[1]Summary!$H53</f>
         <v>17114</v>
       </c>
       <c r="H50" t="s">
@@ -4878,11 +4878,11 @@
         <v>Web Developer Diploma</v>
       </c>
       <c r="B51" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>26.863636363636363</v>
       </c>
       <c r="C51" s="1">
-        <f>[1]Summary!$G54</f>
+        <f ca="1">[1]Summary!$G54</f>
         <v>591</v>
       </c>
       <c r="D51" t="s">
@@ -4896,7 +4896,7 @@
         <v>Diploma</v>
       </c>
       <c r="G51">
-        <f>[1]Summary!$H54</f>
+        <f ca="1">[1]Summary!$H54</f>
         <v>10774</v>
       </c>
       <c r="H51" t="s">

</xml_diff>

<commit_message>
Activate It Tech Support. Fix PC Support
</commit_message>
<xml_diff>
--- a/static/programlisting.xlsx
+++ b/static/programlisting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\aolccbc.com\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1E604E-3D1E-41EC-9337-BFDE1F1E56BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D658CF-91E8-4A95-86A8-969C770C5AA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="30">
   <si>
     <t>NameofProgram</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Diploma</t>
+  </si>
+  <si>
+    <t>PC Support Specialist Diploma</t>
   </si>
 </sst>
 </file>
@@ -722,59 +725,59 @@
       <sheetName val="Reference"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-      <sheetData sheetId="52" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
+      <sheetData sheetId="51"/>
+      <sheetData sheetId="52"/>
       <sheetData sheetId="53">
         <row r="5">
           <cell r="A5" t="str">
@@ -1239,9 +1242,6 @@
           </cell>
         </row>
         <row r="47">
-          <cell r="A47" t="str">
-            <v>PC SUPPORT SPECIALIST DIPLOMA</v>
-          </cell>
           <cell r="G47">
             <v>1164</v>
           </cell>
@@ -2047,8 +2047,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="55" refreshError="1"/>
-      <sheetData sheetId="56" refreshError="1"/>
+      <sheetData sheetId="55"/>
+      <sheetData sheetId="56"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2351,10 +2351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2419,11 +2419,11 @@
         <v>A+ Network+ And Mcsa Desktop Cert. Prep</v>
       </c>
       <c r="B2" s="1">
-        <f t="shared" ref="B2:B33" ca="1" si="0">C2/weeks</f>
+        <f t="shared" ref="B2:B33" si="0">C2/weeks</f>
         <v>34.090909090909093</v>
       </c>
       <c r="C2" s="1">
-        <f ca="1">[1]Summary!$G5</f>
+        <f>[1]Summary!$G5</f>
         <v>750</v>
       </c>
       <c r="D2" t="s">
@@ -2437,7 +2437,7 @@
         <v>Certificate</v>
       </c>
       <c r="G2">
-        <f ca="1">[1]Summary!$H5</f>
+        <f>[1]Summary!$H5</f>
         <v>8510</v>
       </c>
       <c r="H2" t="s">
@@ -2469,11 +2469,11 @@
         <v>Accounting Administrator Diploma With Sage</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>35.863636363636367</v>
       </c>
       <c r="C3" s="1">
-        <f ca="1">[1]Summary!$G6</f>
+        <f>[1]Summary!$G6</f>
         <v>789</v>
       </c>
       <c r="D3" t="s">
@@ -2487,7 +2487,7 @@
         <v>Diploma</v>
       </c>
       <c r="G3">
-        <f ca="1">[1]Summary!$H6</f>
+        <f>[1]Summary!$H6</f>
         <v>11559</v>
       </c>
       <c r="H3" t="s">
@@ -2519,11 +2519,11 @@
         <v>Accounting And Business Technology Diploma</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>40.863636363636367</v>
       </c>
       <c r="C4" s="1">
-        <f ca="1">[1]Summary!$G7</f>
+        <f>[1]Summary!$G7</f>
         <v>899</v>
       </c>
       <c r="D4" t="s">
@@ -2537,7 +2537,7 @@
         <v>Diploma</v>
       </c>
       <c r="G4">
-        <f ca="1">[1]Summary!$H7</f>
+        <f>[1]Summary!$H7</f>
         <v>12729</v>
       </c>
       <c r="H4" t="s">
@@ -2569,11 +2569,11 @@
         <v>Accounting And Payroll Administrator Diploma</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>49.272727272727273</v>
       </c>
       <c r="C5" s="1">
-        <f ca="1">[1]Summary!$G8</f>
+        <f>[1]Summary!$G8</f>
         <v>1084</v>
       </c>
       <c r="D5" t="s">
@@ -2587,7 +2587,7 @@
         <v>Diploma</v>
       </c>
       <c r="G5">
-        <f ca="1">[1]Summary!$H8</f>
+        <f>[1]Summary!$H8</f>
         <v>15180</v>
       </c>
       <c r="H5" t="s">
@@ -2619,11 +2619,11 @@
         <v>Accounting Bookkeeper Certificate</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>29.227272727272727</v>
       </c>
       <c r="C6" s="1">
-        <f ca="1">[1]Summary!$G9</f>
+        <f>[1]Summary!$G9</f>
         <v>643</v>
       </c>
       <c r="D6" t="s">
@@ -2637,7 +2637,7 @@
         <v>Certificate</v>
       </c>
       <c r="G6">
-        <f ca="1">[1]Summary!$H9</f>
+        <f>[1]Summary!$H9</f>
         <v>8707</v>
       </c>
       <c r="H6" t="s">
@@ -2669,11 +2669,11 @@
         <v>Accounting Clerk Certificate</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>20.90909090909091</v>
       </c>
       <c r="C7" s="1">
-        <f ca="1">[1]Summary!$G10</f>
+        <f>[1]Summary!$G10</f>
         <v>460</v>
       </c>
       <c r="D7" t="s">
@@ -2687,7 +2687,7 @@
         <v>Certificate</v>
       </c>
       <c r="G7">
-        <f ca="1">[1]Summary!$H10</f>
+        <f>[1]Summary!$H10</f>
         <v>6452</v>
       </c>
       <c r="H7" t="s">
@@ -2719,11 +2719,11 @@
         <v>Addictions Worker Certificate</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>13.636363636363637</v>
       </c>
       <c r="C8" s="1">
-        <f ca="1">[1]Summary!$G11</f>
+        <f>[1]Summary!$G11</f>
         <v>300</v>
       </c>
       <c r="D8" t="s">
@@ -2737,7 +2737,7 @@
         <v>Certificate</v>
       </c>
       <c r="G8">
-        <f ca="1">[1]Summary!$H11</f>
+        <f>[1]Summary!$H11</f>
         <v>3079</v>
       </c>
       <c r="H8" t="s">
@@ -2769,11 +2769,11 @@
         <v>Administrative Assistant Diploma</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>34.909090909090907</v>
       </c>
       <c r="C9" s="1">
-        <f ca="1">[1]Summary!$G12</f>
+        <f>[1]Summary!$G12</f>
         <v>768</v>
       </c>
       <c r="D9" t="s">
@@ -2787,7 +2787,7 @@
         <v>Diploma</v>
       </c>
       <c r="G9">
-        <f ca="1">[1]Summary!$H12</f>
+        <f>[1]Summary!$H12</f>
         <v>10097</v>
       </c>
       <c r="H9" t="s">
@@ -2819,11 +2819,11 @@
         <v>Business Administration Co-Op Diploma</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>97.13636363636364</v>
       </c>
       <c r="C10" s="1">
-        <f ca="1">[1]Summary!$G13</f>
+        <f>[1]Summary!$G13</f>
         <v>2137</v>
       </c>
       <c r="D10" t="s">
@@ -2837,7 +2837,7 @@
         <v>Diploma</v>
       </c>
       <c r="G10">
-        <f ca="1">[1]Summary!$H13</f>
+        <f>[1]Summary!$H13</f>
         <v>22293</v>
       </c>
       <c r="H10" t="s">
@@ -2869,11 +2869,11 @@
         <v>Business Administration Diploma</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>57.590909090909093</v>
       </c>
       <c r="C11" s="1">
-        <f ca="1">[1]Summary!$G14</f>
+        <f>[1]Summary!$G14</f>
         <v>1267</v>
       </c>
       <c r="D11" t="s">
@@ -2887,7 +2887,7 @@
         <v>Diploma</v>
       </c>
       <c r="G11">
-        <f ca="1">[1]Summary!$H14</f>
+        <f>[1]Summary!$H14</f>
         <v>17893</v>
       </c>
       <c r="H11" t="s">
@@ -2919,11 +2919,11 @@
         <v>Business Management Certificate</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>28.045454545454547</v>
       </c>
       <c r="C12" s="1">
-        <f ca="1">[1]Summary!$G15</f>
+        <f>[1]Summary!$G15</f>
         <v>617</v>
       </c>
       <c r="D12" t="s">
@@ -2937,7 +2937,7 @@
         <v>Certificate</v>
       </c>
       <c r="G12">
-        <f ca="1">[1]Summary!$H15</f>
+        <f>[1]Summary!$H15</f>
         <v>9329</v>
       </c>
       <c r="H12" t="s">
@@ -2969,11 +2969,11 @@
         <v>Business Office Skills Diploma</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>38.31818181818182</v>
       </c>
       <c r="C13" s="1">
-        <f ca="1">[1]Summary!$G16</f>
+        <f>[1]Summary!$G16</f>
         <v>843</v>
       </c>
       <c r="D13" t="s">
@@ -2987,7 +2987,7 @@
         <v>Diploma</v>
       </c>
       <c r="G13">
-        <f ca="1">[1]Summary!$H16</f>
+        <f>[1]Summary!$H16</f>
         <v>11409</v>
       </c>
       <c r="H13" t="s">
@@ -3019,11 +3019,11 @@
         <v>Business Receptionist Certificate</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>24.59090909090909</v>
       </c>
       <c r="C14" s="1">
-        <f ca="1">[1]Summary!$G17</f>
+        <f>[1]Summary!$G17</f>
         <v>541</v>
       </c>
       <c r="D14" t="s">
@@ -3037,7 +3037,7 @@
         <v>Certificate</v>
       </c>
       <c r="G14">
-        <f ca="1">[1]Summary!$H17</f>
+        <f>[1]Summary!$H17</f>
         <v>7135</v>
       </c>
       <c r="H14" t="s">
@@ -3069,11 +3069,11 @@
         <v>Business Service Essentials Co-Op Diploma</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>48.909090909090907</v>
       </c>
       <c r="C15" s="1">
-        <f ca="1">[1]Summary!$G18</f>
+        <f>[1]Summary!$G18</f>
         <v>1076</v>
       </c>
       <c r="D15" t="s">
@@ -3087,7 +3087,7 @@
         <v>Diploma</v>
       </c>
       <c r="G15">
-        <f ca="1">[1]Summary!$H18</f>
+        <f>[1]Summary!$H18</f>
         <v>10752</v>
       </c>
       <c r="H15" t="s">
@@ -3119,11 +3119,11 @@
         <v>Call Centre Customer Representative Diploma</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>31.181818181818183</v>
       </c>
       <c r="C16" s="1">
-        <f ca="1">[1]Summary!$G19</f>
+        <f>[1]Summary!$G19</f>
         <v>686</v>
       </c>
       <c r="D16" t="s">
@@ -3137,7 +3137,7 @@
         <v>Diploma</v>
       </c>
       <c r="G16">
-        <f ca="1">[1]Summary!$H19</f>
+        <f>[1]Summary!$H19</f>
         <v>9627</v>
       </c>
       <c r="H16" t="s">
@@ -3169,11 +3169,11 @@
         <v>Community Service Worker And Addictions Worker Diploma</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>52.590909090909093</v>
       </c>
       <c r="C17" s="1">
-        <f ca="1">[1]Summary!$G20</f>
+        <f>[1]Summary!$G20</f>
         <v>1157</v>
       </c>
       <c r="D17" t="s">
@@ -3187,7 +3187,7 @@
         <v>Diploma</v>
       </c>
       <c r="G17">
-        <f ca="1">[1]Summary!$H20</f>
+        <f>[1]Summary!$H20</f>
         <v>15449</v>
       </c>
       <c r="H17" t="s">
@@ -3219,11 +3219,11 @@
         <v>Community Service Worker Diploma</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>37.590909090909093</v>
       </c>
       <c r="C18" s="1">
-        <f ca="1">[1]Summary!$G21</f>
+        <f>[1]Summary!$G21</f>
         <v>827</v>
       </c>
       <c r="D18" t="s">
@@ -3237,7 +3237,7 @@
         <v>Diploma</v>
       </c>
       <c r="G18">
-        <f ca="1">[1]Summary!$H21</f>
+        <f>[1]Summary!$H21</f>
         <v>12370</v>
       </c>
       <c r="H18" t="s">
@@ -3272,11 +3272,11 @@
         <v>Computer Service Technician Certificate</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>26.636363636363637</v>
       </c>
       <c r="C19" s="1">
-        <f ca="1">[1]Summary!$G22</f>
+        <f>[1]Summary!$G22</f>
         <v>586</v>
       </c>
       <c r="D19" t="s">
@@ -3290,7 +3290,7 @@
         <v>Certificate</v>
       </c>
       <c r="G19">
-        <f ca="1">[1]Summary!$H22</f>
+        <f>[1]Summary!$H22</f>
         <v>5822</v>
       </c>
       <c r="H19" t="s">
@@ -3325,11 +3325,11 @@
         <v>Computer Service Technician Diploma</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>46.31818181818182</v>
       </c>
       <c r="C20" s="1">
-        <f ca="1">[1]Summary!$G23</f>
+        <f>[1]Summary!$G23</f>
         <v>1019</v>
       </c>
       <c r="D20" t="s">
@@ -3343,7 +3343,7 @@
         <v>Diploma</v>
       </c>
       <c r="G20">
-        <f ca="1">[1]Summary!$H23</f>
+        <f>[1]Summary!$H23</f>
         <v>12167</v>
       </c>
       <c r="H20" t="s">
@@ -3378,11 +3378,11 @@
         <v>Computer Software Support Diploma</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>46.31818181818182</v>
       </c>
       <c r="C21" s="1">
-        <f ca="1">[1]Summary!$G24</f>
+        <f>[1]Summary!$G24</f>
         <v>1019</v>
       </c>
       <c r="D21" t="s">
@@ -3396,7 +3396,7 @@
         <v>Diploma</v>
       </c>
       <c r="G21">
-        <f ca="1">[1]Summary!$H24</f>
+        <f>[1]Summary!$H24</f>
         <v>12167</v>
       </c>
       <c r="H21" t="s">
@@ -3428,11 +3428,11 @@
         <v>Computerized Office Procedures Certificate</v>
       </c>
       <c r="B22" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>25.59090909090909</v>
       </c>
       <c r="C22" s="1">
-        <f ca="1">[1]Summary!$G25</f>
+        <f>[1]Summary!$G25</f>
         <v>563</v>
       </c>
       <c r="D22" t="s">
@@ -3446,7 +3446,7 @@
         <v>Certificate</v>
       </c>
       <c r="G22">
-        <f ca="1">[1]Summary!$H25</f>
+        <f>[1]Summary!$H25</f>
         <v>7132</v>
       </c>
       <c r="H22" t="s">
@@ -3478,11 +3478,11 @@
         <v>Conference And Event Planner Diploma</v>
       </c>
       <c r="B23" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>46.227272727272727</v>
       </c>
       <c r="C23" s="1">
-        <f ca="1">[1]Summary!$G26</f>
+        <f>[1]Summary!$G26</f>
         <v>1017</v>
       </c>
       <c r="D23" t="s">
@@ -3496,7 +3496,7 @@
         <v>Diploma</v>
       </c>
       <c r="G23">
-        <f ca="1">[1]Summary!$H26</f>
+        <f>[1]Summary!$H26</f>
         <v>14474</v>
       </c>
       <c r="H23" t="s">
@@ -3528,11 +3528,11 @@
         <v>Customer Service Representative Certificate</v>
       </c>
       <c r="B24" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>20.727272727272727</v>
       </c>
       <c r="C24" s="1">
-        <f ca="1">[1]Summary!$G27</f>
+        <f>[1]Summary!$G27</f>
         <v>456</v>
       </c>
       <c r="D24" t="s">
@@ -3546,7 +3546,7 @@
         <v>Certificate</v>
       </c>
       <c r="G24">
-        <f ca="1">[1]Summary!$H27</f>
+        <f>[1]Summary!$H27</f>
         <v>6271</v>
       </c>
       <c r="H24" t="s">
@@ -3578,11 +3578,11 @@
         <v>English As Second Language</v>
       </c>
       <c r="B25" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>14.545454545454545</v>
       </c>
       <c r="C25" s="1">
-        <f ca="1">[1]Summary!$G28</f>
+        <f>[1]Summary!$G28</f>
         <v>320</v>
       </c>
       <c r="D25" t="s">
@@ -3596,7 +3596,7 @@
         <v>Certificate</v>
       </c>
       <c r="G25">
-        <f ca="1">[1]Summary!$H28</f>
+        <f>[1]Summary!$H28</f>
         <v>3390</v>
       </c>
       <c r="H25" t="s">
@@ -3628,11 +3628,11 @@
         <v>Entrepreneurial Business Applications Diploma</v>
       </c>
       <c r="B26" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>41.18181818181818</v>
       </c>
       <c r="C26" s="1">
-        <f ca="1">[1]Summary!$G29</f>
+        <f>[1]Summary!$G29</f>
         <v>906</v>
       </c>
       <c r="D26" t="s">
@@ -3646,7 +3646,7 @@
         <v>Diploma</v>
       </c>
       <c r="G26">
-        <f ca="1">[1]Summary!$H29</f>
+        <f>[1]Summary!$H29</f>
         <v>12541</v>
       </c>
       <c r="H26" t="s">
@@ -3678,11 +3678,11 @@
         <v>Executive Assistant Diploma</v>
       </c>
       <c r="B27" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>48.136363636363633</v>
       </c>
       <c r="C27" s="1">
-        <f ca="1">[1]Summary!$G30</f>
+        <f>[1]Summary!$G30</f>
         <v>1059</v>
       </c>
       <c r="D27" t="s">
@@ -3696,7 +3696,7 @@
         <v>Diploma</v>
       </c>
       <c r="G27">
-        <f ca="1">[1]Summary!$H30</f>
+        <f>[1]Summary!$H30</f>
         <v>14334</v>
       </c>
       <c r="H27" t="s">
@@ -3728,11 +3728,11 @@
         <v>Graphic Designer Diploma</v>
       </c>
       <c r="B28" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>49.454545454545453</v>
       </c>
       <c r="C28" s="1">
-        <f ca="1">[1]Summary!$G31</f>
+        <f>[1]Summary!$G31</f>
         <v>1088</v>
       </c>
       <c r="D28" t="s">
@@ -3746,7 +3746,7 @@
         <v>Diploma</v>
       </c>
       <c r="G28">
-        <f ca="1">[1]Summary!$H31</f>
+        <f>[1]Summary!$H31</f>
         <v>16396</v>
       </c>
       <c r="H28" t="s">
@@ -3778,11 +3778,11 @@
         <v>Human Resources Administration Certificate</v>
       </c>
       <c r="B29" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>29.09090909090909</v>
       </c>
       <c r="C29" s="1">
-        <f ca="1">[1]Summary!$G32</f>
+        <f>[1]Summary!$G32</f>
         <v>640</v>
       </c>
       <c r="D29" t="s">
@@ -3796,7 +3796,7 @@
         <v>Certificate</v>
       </c>
       <c r="G29">
-        <f ca="1">[1]Summary!$H32</f>
+        <f>[1]Summary!$H32</f>
         <v>8468</v>
       </c>
       <c r="H29" t="s">
@@ -3828,11 +3828,11 @@
         <v>Marketing Administrative Assistant Certificate</v>
       </c>
       <c r="B30" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>34.545454545454547</v>
       </c>
       <c r="C30" s="1">
-        <f ca="1">[1]Summary!$G33</f>
+        <f>[1]Summary!$G33</f>
         <v>760</v>
       </c>
       <c r="D30" t="s">
@@ -3846,7 +3846,7 @@
         <v>Certificate</v>
       </c>
       <c r="G30">
-        <f ca="1">[1]Summary!$H33</f>
+        <f>[1]Summary!$H33</f>
         <v>10655</v>
       </c>
       <c r="H30" t="s">
@@ -3878,11 +3878,11 @@
         <v>Marketing Coordinator Diploma</v>
       </c>
       <c r="B31" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>43.045454545454547</v>
       </c>
       <c r="C31" s="1">
-        <f ca="1">[1]Summary!$G34</f>
+        <f>[1]Summary!$G34</f>
         <v>947</v>
       </c>
       <c r="D31" t="s">
@@ -3896,7 +3896,7 @@
         <v>Diploma</v>
       </c>
       <c r="G31">
-        <f ca="1">[1]Summary!$H34</f>
+        <f>[1]Summary!$H34</f>
         <v>14242</v>
       </c>
       <c r="H31" t="s">
@@ -3928,11 +3928,11 @@
         <v>Medical Administrative Assistant Certificate</v>
       </c>
       <c r="B32" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>39.727272727272727</v>
       </c>
       <c r="C32" s="1">
-        <f ca="1">[1]Summary!$G35</f>
+        <f>[1]Summary!$G35</f>
         <v>874</v>
       </c>
       <c r="D32" t="s">
@@ -3946,7 +3946,7 @@
         <v>Certificate</v>
       </c>
       <c r="G32">
-        <f ca="1">[1]Summary!$H35</f>
+        <f>[1]Summary!$H35</f>
         <v>10875</v>
       </c>
       <c r="H32" t="s">
@@ -3978,11 +3978,11 @@
         <v>Medical Office Assistant Diploma</v>
       </c>
       <c r="B33" s="1">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>45.81818181818182</v>
       </c>
       <c r="C33" s="1">
-        <f ca="1">[1]Summary!$G36</f>
+        <f>[1]Summary!$G36</f>
         <v>1008</v>
       </c>
       <c r="D33" t="s">
@@ -3996,7 +3996,7 @@
         <v>Diploma</v>
       </c>
       <c r="G33">
-        <f ca="1">[1]Summary!$H36</f>
+        <f>[1]Summary!$H36</f>
         <v>14133</v>
       </c>
       <c r="H33" t="s">
@@ -4028,11 +4028,11 @@
         <v>Medical Office Assistant Diploma W/ Unit Clerk</v>
       </c>
       <c r="B34" s="1">
-        <f t="shared" ref="B34:B52" ca="1" si="5">C34/weeks</f>
+        <f t="shared" ref="B34:B52" si="5">C34/weeks</f>
         <v>59.18181818181818</v>
       </c>
       <c r="C34" s="1">
-        <f ca="1">[1]Summary!$G37</f>
+        <f>[1]Summary!$G37</f>
         <v>1302</v>
       </c>
       <c r="D34" t="s">
@@ -4046,7 +4046,7 @@
         <v>Diploma</v>
       </c>
       <c r="G34">
-        <f ca="1">[1]Summary!$H37</f>
+        <f>[1]Summary!$H37</f>
         <v>16455</v>
       </c>
       <c r="H34" t="s">
@@ -4078,11 +4078,11 @@
         <v>Medical Office Front Desk Assistant Certificate</v>
       </c>
       <c r="B35" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>26.09090909090909</v>
       </c>
       <c r="C35" s="1">
-        <f ca="1">[1]Summary!$G38</f>
+        <f>[1]Summary!$G38</f>
         <v>574</v>
       </c>
       <c r="D35" t="s">
@@ -4096,7 +4096,7 @@
         <v>Certificate</v>
       </c>
       <c r="G35">
-        <f ca="1">[1]Summary!$H38</f>
+        <f>[1]Summary!$H38</f>
         <v>7048</v>
       </c>
       <c r="H35" t="s">
@@ -4128,11 +4128,11 @@
         <v>Microsoft Certified Solutions Associate: Server Cert.</v>
       </c>
       <c r="B36" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>18.954545454545453</v>
       </c>
       <c r="C36" s="1">
-        <f ca="1">[1]Summary!$G39</f>
+        <f>[1]Summary!$G39</f>
         <v>417</v>
       </c>
       <c r="D36" t="s">
@@ -4146,7 +4146,7 @@
         <v>Certificate</v>
       </c>
       <c r="G36">
-        <f ca="1">[1]Summary!$H39</f>
+        <f>[1]Summary!$H39</f>
         <v>5624</v>
       </c>
       <c r="H36" t="s">
@@ -4178,11 +4178,11 @@
         <v>Microsoft Certified Solutions Associate: Windows</v>
       </c>
       <c r="B37" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>18.954545454545453</v>
       </c>
       <c r="C37" s="1">
-        <f ca="1">[1]Summary!$G40</f>
+        <f>[1]Summary!$G40</f>
         <v>417</v>
       </c>
       <c r="D37" t="s">
@@ -4196,7 +4196,7 @@
         <v>Certificate</v>
       </c>
       <c r="G37">
-        <f ca="1">[1]Summary!$H40</f>
+        <f>[1]Summary!$H40</f>
         <v>5624</v>
       </c>
       <c r="H37" t="s">
@@ -4228,11 +4228,11 @@
         <v>Network Administrator Diploma (Server 2016)</v>
       </c>
       <c r="B38" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>79.681818181818187</v>
       </c>
       <c r="C38" s="1">
-        <f ca="1">[1]Summary!$G41</f>
+        <f>[1]Summary!$G41</f>
         <v>1753</v>
       </c>
       <c r="D38" t="s">
@@ -4246,7 +4246,7 @@
         <v>Diploma</v>
       </c>
       <c r="G38">
-        <f ca="1">[1]Summary!$H41</f>
+        <f>[1]Summary!$H41</f>
         <v>20916</v>
       </c>
       <c r="H38" t="s">
@@ -4278,11 +4278,11 @@
         <v>Office Administration Assistant Certificate</v>
       </c>
       <c r="B39" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>21.454545454545453</v>
       </c>
       <c r="C39" s="1">
-        <f ca="1">[1]Summary!$G42</f>
+        <f>[1]Summary!$G42</f>
         <v>472</v>
       </c>
       <c r="D39" t="s">
@@ -4296,7 +4296,7 @@
         <v>Certificate</v>
       </c>
       <c r="G39">
-        <f ca="1">[1]Summary!$H42</f>
+        <f>[1]Summary!$H42</f>
         <v>6296</v>
       </c>
       <c r="H39" t="s">
@@ -4328,11 +4328,11 @@
         <v>Office Administration Diploma</v>
       </c>
       <c r="B40" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>48.227272727272727</v>
       </c>
       <c r="C40" s="1">
-        <f ca="1">[1]Summary!$G43</f>
+        <f>[1]Summary!$G43</f>
         <v>1061</v>
       </c>
       <c r="D40" t="s">
@@ -4346,7 +4346,7 @@
         <v>Diploma</v>
       </c>
       <c r="G40">
-        <f ca="1">[1]Summary!$H43</f>
+        <f>[1]Summary!$H43</f>
         <v>14251</v>
       </c>
       <c r="H40" t="s">
@@ -4378,11 +4378,11 @@
         <v>Office Clerk Certificate</v>
       </c>
       <c r="B41" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>19.772727272727273</v>
       </c>
       <c r="C41" s="1">
-        <f ca="1">[1]Summary!$G44</f>
+        <f>[1]Summary!$G44</f>
         <v>435</v>
       </c>
       <c r="D41" t="s">
@@ -4396,7 +4396,7 @@
         <v>Certificate</v>
       </c>
       <c r="G41">
-        <f ca="1">[1]Summary!$H44</f>
+        <f>[1]Summary!$H44</f>
         <v>5487</v>
       </c>
       <c r="H41" t="s">
@@ -4428,11 +4428,11 @@
         <v>Payroll Administrator Certificate</v>
       </c>
       <c r="B42" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>34.227272727272727</v>
       </c>
       <c r="C42" s="1">
-        <f ca="1">[1]Summary!$G45</f>
+        <f>[1]Summary!$G45</f>
         <v>753</v>
       </c>
       <c r="D42" t="s">
@@ -4446,7 +4446,7 @@
         <v>Certificate</v>
       </c>
       <c r="G42">
-        <f ca="1">[1]Summary!$H45</f>
+        <f>[1]Summary!$H45</f>
         <v>10882</v>
       </c>
       <c r="H42" t="s">
@@ -4478,11 +4478,11 @@
         <v>Payroll Clerk Certificate</v>
       </c>
       <c r="B43" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>24.454545454545453</v>
       </c>
       <c r="C43" s="1">
-        <f ca="1">[1]Summary!$G46</f>
+        <f>[1]Summary!$G46</f>
         <v>538</v>
       </c>
       <c r="D43" t="s">
@@ -4496,7 +4496,7 @@
         <v>Certificate</v>
       </c>
       <c r="G43">
-        <f ca="1">[1]Summary!$H46</f>
+        <f>[1]Summary!$H46</f>
         <v>7656</v>
       </c>
       <c r="H43" t="s">
@@ -4523,16 +4523,15 @@
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" t="str">
-        <f>PROPER([1]Summary!$A47)</f>
-        <v>Pc Support Specialist Diploma</v>
+      <c r="A44" t="s">
+        <v>29</v>
       </c>
       <c r="B44" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>52.909090909090907</v>
       </c>
       <c r="C44" s="1">
-        <f ca="1">[1]Summary!$G47</f>
+        <f>[1]Summary!$G47</f>
         <v>1164</v>
       </c>
       <c r="D44" t="s">
@@ -4546,7 +4545,7 @@
         <v>Diploma</v>
       </c>
       <c r="G44">
-        <f ca="1">[1]Summary!$H47</f>
+        <f>[1]Summary!$H47</f>
         <v>13604</v>
       </c>
       <c r="H44" t="s">
@@ -4578,11 +4577,11 @@
         <v>Project Administration Diploma</v>
       </c>
       <c r="B45" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>45.545454545454547</v>
       </c>
       <c r="C45" s="1">
-        <f ca="1">[1]Summary!$G48</f>
+        <f>[1]Summary!$G48</f>
         <v>1002</v>
       </c>
       <c r="D45" t="s">
@@ -4596,7 +4595,7 @@
         <v>Diploma</v>
       </c>
       <c r="G45">
-        <f ca="1">[1]Summary!$H48</f>
+        <f>[1]Summary!$H48</f>
         <v>14175</v>
       </c>
       <c r="H45" t="s">
@@ -4628,11 +4627,11 @@
         <v>Psa - Computerized Office Skills Certificate</v>
       </c>
       <c r="B46" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>10.545454545454545</v>
       </c>
       <c r="C46" s="1">
-        <f ca="1">[1]Summary!$G49</f>
+        <f>[1]Summary!$G49</f>
         <v>232</v>
       </c>
       <c r="D46" t="s">
@@ -4646,7 +4645,7 @@
         <v>Certificate</v>
       </c>
       <c r="G46">
-        <f ca="1">[1]Summary!$H49</f>
+        <f>[1]Summary!$H49</f>
         <v>3471</v>
       </c>
       <c r="H46" t="s">
@@ -4678,11 +4677,11 @@
         <v>Sales Associate Certificate</v>
       </c>
       <c r="B47" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>18.363636363636363</v>
       </c>
       <c r="C47" s="1">
-        <f ca="1">[1]Summary!$G50</f>
+        <f>[1]Summary!$G50</f>
         <v>404</v>
       </c>
       <c r="D47" t="s">
@@ -4696,7 +4695,7 @@
         <v>Certificate</v>
       </c>
       <c r="G47">
-        <f ca="1">[1]Summary!$H50</f>
+        <f>[1]Summary!$H50</f>
         <v>5651</v>
       </c>
       <c r="H47" t="s">
@@ -4728,11 +4727,11 @@
         <v>Sales Professional Diploma</v>
       </c>
       <c r="B48" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>38.363636363636367</v>
       </c>
       <c r="C48" s="1">
-        <f ca="1">[1]Summary!$G51</f>
+        <f>[1]Summary!$G51</f>
         <v>844</v>
       </c>
       <c r="D48" t="s">
@@ -4746,7 +4745,7 @@
         <v>Diploma</v>
       </c>
       <c r="G48">
-        <f ca="1">[1]Summary!$H51</f>
+        <f>[1]Summary!$H51</f>
         <v>11787</v>
       </c>
       <c r="H48" t="s">
@@ -4778,11 +4777,11 @@
         <v>Software And Web Developer Diploma</v>
       </c>
       <c r="B49" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>43.136363636363633</v>
       </c>
       <c r="C49" s="1">
-        <f ca="1">[1]Summary!$G52</f>
+        <f>[1]Summary!$G52</f>
         <v>949</v>
       </c>
       <c r="D49" t="s">
@@ -4796,7 +4795,7 @@
         <v>Diploma</v>
       </c>
       <c r="G49">
-        <f ca="1">[1]Summary!$H52</f>
+        <f>[1]Summary!$H52</f>
         <v>17063</v>
       </c>
       <c r="H49" t="s">
@@ -4828,11 +4827,11 @@
         <v>Web Designer Diploma</v>
       </c>
       <c r="B50" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>53.772727272727273</v>
       </c>
       <c r="C50" s="1">
-        <f ca="1">[1]Summary!$G53</f>
+        <f>[1]Summary!$G53</f>
         <v>1183</v>
       </c>
       <c r="D50" t="s">
@@ -4846,7 +4845,7 @@
         <v>Diploma</v>
       </c>
       <c r="G50">
-        <f ca="1">[1]Summary!$H53</f>
+        <f>[1]Summary!$H53</f>
         <v>17114</v>
       </c>
       <c r="H50" t="s">
@@ -4878,11 +4877,11 @@
         <v>Web Developer Diploma</v>
       </c>
       <c r="B51" s="1">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>26.863636363636363</v>
       </c>
       <c r="C51" s="1">
-        <f ca="1">[1]Summary!$G54</f>
+        <f>[1]Summary!$G54</f>
         <v>591</v>
       </c>
       <c r="D51" t="s">
@@ -4896,7 +4895,7 @@
         <v>Diploma</v>
       </c>
       <c r="G51">
-        <f ca="1">[1]Summary!$H54</f>
+        <f>[1]Summary!$H54</f>
         <v>10774</v>
       </c>
       <c r="H51" t="s">
@@ -4946,7 +4945,7 @@
         <v>20000</v>
       </c>
       <c r="H52" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="I52" t="s">
         <v>14</v>
@@ -4966,12 +4965,6 @@
       <c r="N52" t="str">
         <f t="shared" si="4"/>
         <v>it_tech_support_specialist_diploma.pdf</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" t="str">
-        <f>PROPER([1]Summary!$A56)</f>
-        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated template, src to allow for rm programs
</commit_message>
<xml_diff>
--- a/static/programlisting.xlsx
+++ b/static/programlisting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\aolccbc.com\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E24FA34-DB95-4FFB-A118-419288E049BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDE8769-9A79-4281-9369-233C7DFFCFB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="32">
   <si>
     <t>NameofProgram</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Business</t>
   </si>
   <si>
-    <t>move *csw_with_aw*.pdf community_service_worker_and_addictions_worker_diploma.pdf</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
@@ -118,6 +115,15 @@
   </si>
   <si>
     <t>PC Support Specialist Diploma</t>
+  </si>
+  <si>
+    <t>onsite</t>
+  </si>
+  <si>
+    <t>remote</t>
+  </si>
+  <si>
+    <t>blended</t>
   </si>
 </sst>
 </file>
@@ -2351,10 +2357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="M51" workbookViewId="0">
+      <selection activeCell="R52" sqref="R52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2369,7 +2375,7 @@
     <col min="14" max="14" width="70.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2401,7 +2407,7 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L1" t="s">
         <v>10</v>
@@ -2412,8 +2418,17 @@
       <c r="N1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>PROPER([1]Summary!$A5)</f>
         <v>A+ Network+ And Mcsa Desktop Cert. Prep</v>
@@ -2462,8 +2477,17 @@
         <f>_xlfn.CONCAT(L2,".pdf")</f>
         <v>a_network_and_mcsa_desktop_cert_prep.pdf</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>PROPER([1]Summary!$A6)</f>
         <v>Accounting Administrator Diploma With Sage</v>
@@ -2512,8 +2536,17 @@
         <f t="shared" ref="N3:N52" si="4">_xlfn.CONCAT(L3,"_",LOWER(F3),".pdf")</f>
         <v>accounting_administrator_with_sage_diploma.pdf</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>PROPER([1]Summary!$A7)</f>
         <v>Accounting And Business Technology Diploma</v>
@@ -2562,8 +2595,17 @@
         <f t="shared" si="4"/>
         <v>accounting_and_business_technology_diploma.pdf</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>PROPER([1]Summary!$A8)</f>
         <v>Accounting And Payroll Administrator Diploma</v>
@@ -2612,8 +2654,17 @@
         <f t="shared" si="4"/>
         <v>accounting_and_payroll_administrator_diploma.pdf</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>PROPER([1]Summary!$A9)</f>
         <v>Accounting Bookkeeper Certificate</v>
@@ -2662,8 +2713,17 @@
         <f t="shared" si="4"/>
         <v>accounting_bookkeeper_certificate.pdf</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>PROPER([1]Summary!$A10)</f>
         <v>Accounting Clerk Certificate</v>
@@ -2712,8 +2772,17 @@
         <f t="shared" si="4"/>
         <v>accounting_clerk_certificate.pdf</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>PROPER([1]Summary!$A11)</f>
         <v>Addictions Worker Certificate</v>
@@ -2762,8 +2831,17 @@
         <f t="shared" si="4"/>
         <v>addictions_worker_certificate.pdf</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>PROPER([1]Summary!$A12)</f>
         <v>Administrative Assistant Diploma</v>
@@ -2812,8 +2890,17 @@
         <f t="shared" si="4"/>
         <v>administrative_assistant_diploma.pdf</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>PROPER([1]Summary!$A13)</f>
         <v>Business Administration Co-Op Diploma</v>
@@ -2862,8 +2949,17 @@
         <f t="shared" si="4"/>
         <v>business_administration_co_op_diploma.pdf</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>PROPER([1]Summary!$A14)</f>
         <v>Business Administration Diploma</v>
@@ -2912,8 +3008,17 @@
         <f t="shared" si="4"/>
         <v>business_administration_diploma.pdf</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>PROPER([1]Summary!$A15)</f>
         <v>Business Management Certificate</v>
@@ -2962,8 +3067,17 @@
         <f t="shared" si="4"/>
         <v>business_management_certificate.pdf</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>PROPER([1]Summary!$A16)</f>
         <v>Business Office Skills Diploma</v>
@@ -3012,8 +3126,17 @@
         <f t="shared" si="4"/>
         <v>business_office_skills_diploma.pdf</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>PROPER([1]Summary!$A17)</f>
         <v>Business Receptionist Certificate</v>
@@ -3062,8 +3185,17 @@
         <f t="shared" si="4"/>
         <v>business_receptionist_certificate.pdf</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>PROPER([1]Summary!$A18)</f>
         <v>Business Service Essentials Co-Op Diploma</v>
@@ -3112,8 +3244,17 @@
         <f t="shared" si="4"/>
         <v>business_service_essentials_co_op_diploma.pdf</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>PROPER([1]Summary!$A19)</f>
         <v>Call Centre Customer Representative Diploma</v>
@@ -3162,8 +3303,17 @@
         <f t="shared" si="4"/>
         <v>call_centre_customer_representative_diploma.pdf</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>PROPER([1]Summary!$A20)</f>
         <v>Community Service Worker And Addictions Worker Diploma</v>
@@ -3212,8 +3362,17 @@
         <f t="shared" si="4"/>
         <v>community_service_worker_and_addictions_worker_diploma.pdf</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>PROPER([1]Summary!$A21)</f>
         <v>Community Service Worker Diploma</v>
@@ -3262,11 +3421,17 @@
         <f t="shared" si="4"/>
         <v>community_service_worker_diploma.pdf</v>
       </c>
-      <c r="O18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>PROPER([1]Summary!$A22)</f>
         <v>Computer Service Technician Certificate</v>
@@ -3304,7 +3469,7 @@
         <v>COMPUTER SERVICE TECHNICIAN</v>
       </c>
       <c r="K19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="3"/>
@@ -3318,8 +3483,17 @@
         <f t="shared" si="4"/>
         <v>computer_service_technician_c_certificate.pdf</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>PROPER([1]Summary!$A23)</f>
         <v>Computer Service Technician Diploma</v>
@@ -3357,7 +3531,7 @@
         <v>COMPUTER SERVICE TECHNICIAN</v>
       </c>
       <c r="K20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="3"/>
@@ -3371,8 +3545,17 @@
         <f t="shared" si="4"/>
         <v>computer_service_technician_d_diploma.pdf</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>PROPER([1]Summary!$A24)</f>
         <v>Computer Software Support Diploma</v>
@@ -3400,7 +3583,7 @@
         <v>12167</v>
       </c>
       <c r="H21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I21" t="s">
         <v>14</v>
@@ -3421,8 +3604,17 @@
         <f t="shared" si="4"/>
         <v>computer_software_support_diploma.pdf</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>PROPER([1]Summary!$A25)</f>
         <v>Computerized Office Procedures Certificate</v>
@@ -3471,8 +3663,17 @@
         <f t="shared" si="4"/>
         <v>computerized_office_procedures_certificate.pdf</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>PROPER([1]Summary!$A26)</f>
         <v>Conference And Event Planner Diploma</v>
@@ -3521,8 +3722,17 @@
         <f t="shared" si="4"/>
         <v>conference_and_event_planner_diploma.pdf</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>PROPER([1]Summary!$A27)</f>
         <v>Customer Service Representative Certificate</v>
@@ -3571,8 +3781,17 @@
         <f t="shared" si="4"/>
         <v>customer_service_representative_certificate.pdf</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>PROPER([1]Summary!$A28)</f>
         <v>English As Second Language</v>
@@ -3603,7 +3822,7 @@
         <v>13</v>
       </c>
       <c r="I25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="2"/>
@@ -3621,8 +3840,17 @@
         <f t="shared" si="4"/>
         <v>english_as_second_language_certificate.pdf</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>PROPER([1]Summary!$A29)</f>
         <v>Entrepreneurial Business Applications Diploma</v>
@@ -3671,8 +3899,17 @@
         <f t="shared" si="4"/>
         <v>entrepreneurial_business_applications_diploma.pdf</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>PROPER([1]Summary!$A30)</f>
         <v>Executive Assistant Diploma</v>
@@ -3721,8 +3958,17 @@
         <f t="shared" si="4"/>
         <v>executive_assistant_diploma.pdf</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>PROPER([1]Summary!$A31)</f>
         <v>Graphic Designer Diploma</v>
@@ -3753,7 +3999,7 @@
         <v>13</v>
       </c>
       <c r="I28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="2"/>
@@ -3771,8 +4017,17 @@
         <f t="shared" si="4"/>
         <v>graphic_designer_diploma.pdf</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>PROPER([1]Summary!$A32)</f>
         <v>Human Resources Administration Certificate</v>
@@ -3821,8 +4076,17 @@
         <f t="shared" si="4"/>
         <v>human_resources_administration_certificate.pdf</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>PROPER([1]Summary!$A33)</f>
         <v>Marketing Administrative Assistant Certificate</v>
@@ -3853,7 +4117,7 @@
         <v>13</v>
       </c>
       <c r="I30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" si="2"/>
@@ -3871,8 +4135,17 @@
         <f t="shared" si="4"/>
         <v>marketing_administrative_assistant_certificate.pdf</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O30">
+        <v>1</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>PROPER([1]Summary!$A34)</f>
         <v>Marketing Coordinator Diploma</v>
@@ -3903,7 +4176,7 @@
         <v>13</v>
       </c>
       <c r="I31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" si="2"/>
@@ -3921,8 +4194,17 @@
         <f t="shared" si="4"/>
         <v>marketing_coordinator_diploma.pdf</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>PROPER([1]Summary!$A35)</f>
         <v>Medical Administrative Assistant Certificate</v>
@@ -3953,7 +4235,7 @@
         <v>13</v>
       </c>
       <c r="I32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J32" t="str">
         <f t="shared" si="2"/>
@@ -3971,8 +4253,17 @@
         <f t="shared" si="4"/>
         <v>medical_administrative_assistant_certificate.pdf</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32">
+        <v>1</v>
+      </c>
+      <c r="Q32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>PROPER([1]Summary!$A36)</f>
         <v>Medical Office Assistant Diploma</v>
@@ -4003,7 +4294,7 @@
         <v>13</v>
       </c>
       <c r="I33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J33" t="str">
         <f t="shared" si="2"/>
@@ -4021,8 +4312,17 @@
         <f t="shared" si="4"/>
         <v>medical_office_assistant_diploma.pdf</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33">
+        <v>1</v>
+      </c>
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>PROPER([1]Summary!$A37)</f>
         <v>Medical Office Assistant Diploma W/ Unit Clerk</v>
@@ -4053,7 +4353,7 @@
         <v>13</v>
       </c>
       <c r="I34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J34" t="str">
         <f t="shared" si="2"/>
@@ -4071,8 +4371,17 @@
         <f t="shared" si="4"/>
         <v>medical_office_assistant_w_unit_clerk_diploma.pdf</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34">
+        <v>1</v>
+      </c>
+      <c r="P34">
+        <v>1</v>
+      </c>
+      <c r="Q34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>PROPER([1]Summary!$A38)</f>
         <v>Medical Office Front Desk Assistant Certificate</v>
@@ -4100,10 +4409,10 @@
         <v>7048</v>
       </c>
       <c r="H35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J35" t="str">
         <f t="shared" si="2"/>
@@ -4121,8 +4430,17 @@
         <f t="shared" si="4"/>
         <v>medical_office_front_desk_assistant_certificate.pdf</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35">
+        <v>1</v>
+      </c>
+      <c r="P35">
+        <v>1</v>
+      </c>
+      <c r="Q35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>PROPER([1]Summary!$A39)</f>
         <v>Microsoft Certified Solutions Associate: Server Cert.</v>
@@ -4171,8 +4489,17 @@
         <f t="shared" si="4"/>
         <v>microsoft_certified_solutions_associate_server_cert__certificate.pdf</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36">
+        <v>1</v>
+      </c>
+      <c r="P36">
+        <v>1</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>PROPER([1]Summary!$A40)</f>
         <v>Microsoft Certified Solutions Associate: Windows</v>
@@ -4200,7 +4527,7 @@
         <v>5624</v>
       </c>
       <c r="H37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I37" t="s">
         <v>14</v>
@@ -4221,8 +4548,17 @@
         <f t="shared" si="4"/>
         <v>microsoft_certified_solutions_associate_windows_certificate.pdf</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37">
+        <v>1</v>
+      </c>
+      <c r="P37">
+        <v>1</v>
+      </c>
+      <c r="Q37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>PROPER([1]Summary!$A41)</f>
         <v>Network Administrator Diploma (Server 2016)</v>
@@ -4271,8 +4607,17 @@
         <f t="shared" si="4"/>
         <v>network_administrator_server_2016_diploma.pdf</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38">
+        <v>1</v>
+      </c>
+      <c r="P38">
+        <v>1</v>
+      </c>
+      <c r="Q38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>PROPER([1]Summary!$A42)</f>
         <v>Office Administration Assistant Certificate</v>
@@ -4321,8 +4666,17 @@
         <f t="shared" si="4"/>
         <v>office_administration_assistant_certificate.pdf</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39">
+        <v>1</v>
+      </c>
+      <c r="P39">
+        <v>1</v>
+      </c>
+      <c r="Q39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>PROPER([1]Summary!$A43)</f>
         <v>Office Administration Diploma</v>
@@ -4371,8 +4725,17 @@
         <f t="shared" si="4"/>
         <v>office_administration_diploma.pdf</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40">
+        <v>1</v>
+      </c>
+      <c r="P40">
+        <v>1</v>
+      </c>
+      <c r="Q40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>PROPER([1]Summary!$A44)</f>
         <v>Office Clerk Certificate</v>
@@ -4421,8 +4784,17 @@
         <f t="shared" si="4"/>
         <v>office_clerk_certificate.pdf</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41">
+        <v>1</v>
+      </c>
+      <c r="P41">
+        <v>1</v>
+      </c>
+      <c r="Q41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>PROPER([1]Summary!$A45)</f>
         <v>Payroll Administrator Certificate</v>
@@ -4471,8 +4843,17 @@
         <f t="shared" si="4"/>
         <v>payroll_administrator_certificate.pdf</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42">
+        <v>1</v>
+      </c>
+      <c r="P42">
+        <v>1</v>
+      </c>
+      <c r="Q42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>PROPER([1]Summary!$A46)</f>
         <v>Payroll Clerk Certificate</v>
@@ -4521,10 +4902,19 @@
         <f t="shared" si="4"/>
         <v>payroll_clerk_certificate.pdf</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43">
+        <v>1</v>
+      </c>
+      <c r="P43">
+        <v>1</v>
+      </c>
+      <c r="Q43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B44" s="1">
         <f t="shared" si="5"/>
@@ -4570,8 +4960,17 @@
         <f t="shared" si="4"/>
         <v>pc_support_specialist_diploma.pdf</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44">
+        <v>1</v>
+      </c>
+      <c r="P44">
+        <v>1</v>
+      </c>
+      <c r="Q44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>PROPER([1]Summary!$A48)</f>
         <v>Project Administration Diploma</v>
@@ -4620,8 +5019,17 @@
         <f t="shared" si="4"/>
         <v>project_administration_diploma.pdf</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O45">
+        <v>1</v>
+      </c>
+      <c r="P45">
+        <v>1</v>
+      </c>
+      <c r="Q45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>PROPER([1]Summary!$A49)</f>
         <v>Psa - Computerized Office Skills Certificate</v>
@@ -4649,7 +5057,7 @@
         <v>3471</v>
       </c>
       <c r="H46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I46" t="s">
         <v>17</v>
@@ -4670,8 +5078,17 @@
         <f t="shared" si="4"/>
         <v>psa_computerized_office_skills_certificate.pdf</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46">
+        <v>1</v>
+      </c>
+      <c r="P46">
+        <v>1</v>
+      </c>
+      <c r="Q46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>PROPER([1]Summary!$A50)</f>
         <v>Sales Associate Certificate</v>
@@ -4720,8 +5137,17 @@
         <f t="shared" si="4"/>
         <v>sales_associate_certificate.pdf</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47">
+        <v>1</v>
+      </c>
+      <c r="P47">
+        <v>1</v>
+      </c>
+      <c r="Q47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>PROPER([1]Summary!$A51)</f>
         <v>Sales Professional Diploma</v>
@@ -4770,8 +5196,17 @@
         <f t="shared" si="4"/>
         <v>sales_professional_diploma.pdf</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48">
+        <v>1</v>
+      </c>
+      <c r="P48">
+        <v>1</v>
+      </c>
+      <c r="Q48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>PROPER([1]Summary!$A52)</f>
         <v>Software And Web Developer Diploma</v>
@@ -4802,7 +5237,7 @@
         <v>13</v>
       </c>
       <c r="I49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J49" t="str">
         <f t="shared" si="2"/>
@@ -4820,8 +5255,17 @@
         <f t="shared" si="4"/>
         <v>software_and_web_developer_diploma.pdf</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49">
+        <v>1</v>
+      </c>
+      <c r="P49">
+        <v>1</v>
+      </c>
+      <c r="Q49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>PROPER([1]Summary!$A53)</f>
         <v>Web Designer Diploma</v>
@@ -4852,7 +5296,7 @@
         <v>13</v>
       </c>
       <c r="I50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J50" t="str">
         <f t="shared" si="2"/>
@@ -4870,8 +5314,17 @@
         <f t="shared" si="4"/>
         <v>web_designer_diploma.pdf</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50">
+        <v>1</v>
+      </c>
+      <c r="P50">
+        <v>1</v>
+      </c>
+      <c r="Q50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>PROPER([1]Summary!$A54)</f>
         <v>Web Developer Diploma</v>
@@ -4902,7 +5355,7 @@
         <v>13</v>
       </c>
       <c r="I51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J51" t="str">
         <f t="shared" si="2"/>
@@ -4920,10 +5373,19 @@
         <f t="shared" si="4"/>
         <v>web_developer_diploma.pdf</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51">
+        <v>1</v>
+      </c>
+      <c r="P51">
+        <v>1</v>
+      </c>
+      <c r="Q51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B52" s="1">
         <f t="shared" si="5"/>
@@ -4939,7 +5401,7 @@
         <v>13</v>
       </c>
       <c r="F52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G52">
         <v>16079</v>
@@ -4965,6 +5427,15 @@
       <c r="N52" t="str">
         <f t="shared" si="4"/>
         <v>it_tech_support_specialist_diploma.pdf</v>
+      </c>
+      <c r="O52">
+        <v>0</v>
+      </c>
+      <c r="P52">
+        <v>1</v>
+      </c>
+      <c r="Q52">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5028,22 +5499,22 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>